<commit_message>
Editar lineas de produccion
</commit_message>
<xml_diff>
--- a/Horas de trabajo.xlsx
+++ b/Horas de trabajo.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
   <si>
     <t>HOJA DE HORAS DE TRABAJO PROYECTO CENTROS DE COSTOS</t>
   </si>
@@ -98,7 +98,10 @@
     <t>DOMINGO</t>
   </si>
   <si>
-    <t>TOTAL</t>
+    <t>13/7/2015</t>
+  </si>
+  <si>
+    <t>Se agregó la vista para editar las lineas de producción y se corrigieron links que no estaban funcionando correctamente</t>
   </si>
 </sst>
 </file>
@@ -142,7 +145,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -158,7 +161,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -167,10 +170,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -454,8 +460,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -512,24 +518,24 @@
       <c r="D5" s="7">
         <v>4</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E5" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="8"/>
       <c r="B6" s="8"/>
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
@@ -542,24 +548,24 @@
       <c r="D7" s="7">
         <v>4</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
@@ -572,24 +578,24 @@
       <c r="D9" s="7">
         <v>3</v>
       </c>
-      <c r="E9" s="9" t="s">
+      <c r="E9" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="8"/>
       <c r="B10" s="8"/>
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
@@ -602,13 +608,13 @@
       <c r="D11" s="3">
         <v>3</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="E11" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
     </row>
     <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
@@ -621,35 +627,35 @@
       <c r="D12" s="7">
         <v>8</v>
       </c>
-      <c r="E12" s="9" t="s">
+      <c r="E12" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="8"/>
       <c r="B13" s="8"/>
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="9"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="8"/>
       <c r="B14" s="8"/>
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="9"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
@@ -662,13 +668,13 @@
       <c r="D15" s="4">
         <v>4</v>
       </c>
-      <c r="E15" s="10" t="s">
+      <c r="E15" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="10"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
     </row>
     <row r="16" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
@@ -681,35 +687,35 @@
       <c r="D16" s="7">
         <v>4</v>
       </c>
-      <c r="E16" s="6" t="s">
+      <c r="E16" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="11"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="8"/>
       <c r="B17" s="8"/>
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="11"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="8"/>
       <c r="B18" s="8"/>
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="6"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11"/>
     </row>
     <row r="19" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="8">
@@ -722,24 +728,24 @@
       <c r="D19" s="7">
         <v>4</v>
       </c>
-      <c r="E19" s="9" t="s">
+      <c r="E19" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="9"/>
-      <c r="I19" s="9"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="10"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="8"/>
       <c r="B20" s="8"/>
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
-      <c r="H20" s="9"/>
-      <c r="I20" s="9"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="10"/>
     </row>
     <row r="21" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="8">
@@ -752,24 +758,24 @@
       <c r="D21" s="7">
         <v>4</v>
       </c>
-      <c r="E21" s="6" t="s">
+      <c r="E21" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="11"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="8"/>
       <c r="B22" s="8"/>
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="6"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="11"/>
     </row>
     <row r="23" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="8">
@@ -782,59 +788,62 @@
       <c r="D23" s="7">
         <v>8</v>
       </c>
-      <c r="E23" s="6" t="s">
+      <c r="E23" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="6"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="11"/>
+      <c r="I23" s="11"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="8"/>
       <c r="B24" s="8"/>
       <c r="C24" s="7"/>
       <c r="D24" s="7"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="6"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="11"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="8"/>
       <c r="B25" s="8"/>
       <c r="C25" s="7"/>
       <c r="D25" s="7"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
-      <c r="I25" s="6"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="11"/>
+      <c r="I25" s="11"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26" s="7"/>
+      <c r="C26" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" s="6">
+        <v>4</v>
+      </c>
+      <c r="E26" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C28" t="s">
-        <v>24</v>
-      </c>
-      <c r="D28" s="5">
-        <f>SUM(D5:D25)</f>
-        <v>46</v>
-      </c>
+      <c r="D28" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="39">
-    <mergeCell ref="A19:B20"/>
-    <mergeCell ref="A16:B18"/>
-    <mergeCell ref="E23:I25"/>
-    <mergeCell ref="D23:D25"/>
-    <mergeCell ref="C23:C25"/>
-    <mergeCell ref="A23:B25"/>
-    <mergeCell ref="E16:I18"/>
-    <mergeCell ref="D16:D18"/>
-    <mergeCell ref="C16:C18"/>
-    <mergeCell ref="E19:I20"/>
+  <mergeCells count="40">
+    <mergeCell ref="A21:B22"/>
     <mergeCell ref="D19:D20"/>
     <mergeCell ref="C19:C20"/>
+    <mergeCell ref="E21:I22"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="C21:C22"/>
     <mergeCell ref="A7:B8"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="E11:I11"/>
@@ -846,10 +855,6 @@
     <mergeCell ref="E7:I8"/>
     <mergeCell ref="D7:D8"/>
     <mergeCell ref="C7:C8"/>
-    <mergeCell ref="E21:I22"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="A21:B22"/>
     <mergeCell ref="A3:B4"/>
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="E4:I4"/>
@@ -857,11 +862,22 @@
     <mergeCell ref="D5:D6"/>
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="A5:B6"/>
+    <mergeCell ref="A26:B26"/>
     <mergeCell ref="A15:B15"/>
     <mergeCell ref="E15:I15"/>
     <mergeCell ref="A9:B10"/>
     <mergeCell ref="C9:C10"/>
     <mergeCell ref="D9:D10"/>
+    <mergeCell ref="A19:B20"/>
+    <mergeCell ref="A16:B18"/>
+    <mergeCell ref="E23:I25"/>
+    <mergeCell ref="D23:D25"/>
+    <mergeCell ref="C23:C25"/>
+    <mergeCell ref="A23:B25"/>
+    <mergeCell ref="E16:I18"/>
+    <mergeCell ref="D16:D18"/>
+    <mergeCell ref="C16:C18"/>
+    <mergeCell ref="E19:I20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Editar materiales y categorias
</commit_message>
<xml_diff>
--- a/Horas de trabajo.xlsx
+++ b/Horas de trabajo.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
   <si>
     <t>HOJA DE HORAS DE TRABAJO PROYECTO CENTROS DE COSTOS</t>
   </si>
@@ -102,6 +102,15 @@
   </si>
   <si>
     <t>Se agregó la vista para editar las lineas de producción y se corrigieron links que no estaban funcionando correctamente</t>
+  </si>
+  <si>
+    <t>15/7/2015</t>
+  </si>
+  <si>
+    <t>MIERCOLES</t>
+  </si>
+  <si>
+    <t>Añadida funcionalidad para editar materiales y categorias. Los materiales mantienen su costo, el cual va a corresponder a su descripcion</t>
   </si>
 </sst>
 </file>
@@ -145,15 +154,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -170,13 +173,16 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -460,13 +466,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27:B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="75" customWidth="1"/>
   </cols>
   <sheetData>
@@ -508,10 +515,10 @@
       <c r="I4" s="7"/>
     </row>
     <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="8"/>
+      <c r="B5" s="6"/>
       <c r="C5" s="7" t="s">
         <v>6</v>
       </c>
@@ -527,8 +534,8 @@
       <c r="I5" s="10"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="8"/>
-      <c r="B6" s="8"/>
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
       <c r="E6" s="10"/>
@@ -568,10 +575,10 @@
       <c r="I8" s="10"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="8">
+      <c r="A9" s="6">
         <v>42042</v>
       </c>
-      <c r="B9" s="8"/>
+      <c r="B9" s="6"/>
       <c r="C9" s="7" t="s">
         <v>12</v>
       </c>
@@ -587,8 +594,8 @@
       <c r="I9" s="10"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="8"/>
-      <c r="B10" s="8"/>
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
       <c r="E10" s="10"/>
@@ -598,7 +605,7 @@
       <c r="I10" s="10"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="8">
+      <c r="A11" s="6">
         <v>42070</v>
       </c>
       <c r="B11" s="7"/>
@@ -617,10 +624,10 @@
       <c r="I11" s="9"/>
     </row>
     <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="8">
+      <c r="A12" s="6">
         <v>42101</v>
       </c>
-      <c r="B12" s="8"/>
+      <c r="B12" s="6"/>
       <c r="C12" s="7" t="s">
         <v>16</v>
       </c>
@@ -636,8 +643,8 @@
       <c r="I12" s="10"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="8"/>
-      <c r="B13" s="8"/>
+      <c r="A13" s="6"/>
+      <c r="B13" s="6"/>
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
       <c r="E13" s="10"/>
@@ -647,8 +654,8 @@
       <c r="I13" s="10"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="8"/>
-      <c r="B14" s="8"/>
+      <c r="A14" s="6"/>
+      <c r="B14" s="6"/>
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
       <c r="E14" s="10"/>
@@ -658,7 +665,7 @@
       <c r="I14" s="10"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="8">
+      <c r="A15" s="6">
         <v>42162</v>
       </c>
       <c r="B15" s="7"/>
@@ -677,51 +684,51 @@
       <c r="I15" s="9"/>
     </row>
     <row r="16" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="8">
+      <c r="A16" s="6">
         <v>42192</v>
       </c>
-      <c r="B16" s="8"/>
+      <c r="B16" s="6"/>
       <c r="C16" s="7" t="s">
         <v>10</v>
       </c>
       <c r="D16" s="7">
         <v>4</v>
       </c>
-      <c r="E16" s="11" t="s">
+      <c r="E16" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="11"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="8"/>
-      <c r="B17" s="8"/>
+      <c r="A17" s="6"/>
+      <c r="B17" s="6"/>
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="11"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="8"/>
-      <c r="B18" s="8"/>
+      <c r="A18" s="6"/>
+      <c r="B18" s="6"/>
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="11"/>
-      <c r="I18" s="11"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
     </row>
     <row r="19" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="8">
+      <c r="A19" s="6">
         <v>42284</v>
       </c>
-      <c r="B19" s="8"/>
+      <c r="B19" s="6"/>
       <c r="C19" s="7" t="s">
         <v>14</v>
       </c>
@@ -737,8 +744,8 @@
       <c r="I19" s="10"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="8"/>
-      <c r="B20" s="8"/>
+      <c r="A20" s="6"/>
+      <c r="B20" s="6"/>
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
       <c r="E20" s="10"/>
@@ -748,120 +755,127 @@
       <c r="I20" s="10"/>
     </row>
     <row r="21" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="8">
+      <c r="A21" s="6">
         <v>42315</v>
       </c>
-      <c r="B21" s="8"/>
+      <c r="B21" s="6"/>
       <c r="C21" s="7" t="s">
         <v>16</v>
       </c>
       <c r="D21" s="7">
         <v>4</v>
       </c>
-      <c r="E21" s="11" t="s">
+      <c r="E21" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="F21" s="11"/>
-      <c r="G21" s="11"/>
-      <c r="H21" s="11"/>
-      <c r="I21" s="11"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="8"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="8"/>
-      <c r="B22" s="8"/>
+      <c r="A22" s="6"/>
+      <c r="B22" s="6"/>
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="11"/>
-      <c r="H22" s="11"/>
-      <c r="I22" s="11"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
     </row>
     <row r="23" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="8">
+      <c r="A23" s="6">
         <v>42345</v>
       </c>
-      <c r="B23" s="8"/>
+      <c r="B23" s="6"/>
       <c r="C23" s="7" t="s">
         <v>23</v>
       </c>
       <c r="D23" s="7">
         <v>8</v>
       </c>
-      <c r="E23" s="11" t="s">
+      <c r="E23" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="F23" s="11"/>
-      <c r="G23" s="11"/>
-      <c r="H23" s="11"/>
-      <c r="I23" s="11"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="8"/>
-      <c r="B24" s="8"/>
+      <c r="A24" s="6"/>
+      <c r="B24" s="6"/>
       <c r="C24" s="7"/>
       <c r="D24" s="7"/>
-      <c r="E24" s="11"/>
-      <c r="F24" s="11"/>
-      <c r="G24" s="11"/>
-      <c r="H24" s="11"/>
-      <c r="I24" s="11"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="8"/>
+      <c r="I24" s="8"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="8"/>
-      <c r="B25" s="8"/>
+      <c r="A25" s="6"/>
+      <c r="B25" s="6"/>
       <c r="C25" s="7"/>
       <c r="D25" s="7"/>
-      <c r="E25" s="11"/>
-      <c r="F25" s="11"/>
-      <c r="G25" s="11"/>
-      <c r="H25" s="11"/>
-      <c r="I25" s="11"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="8"/>
+      <c r="I25" s="8"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>24</v>
       </c>
       <c r="B26" s="7"/>
-      <c r="C26" s="6" t="s">
+      <c r="C26" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D26" s="6">
+      <c r="D26" s="5">
         <v>4</v>
       </c>
       <c r="E26" t="s">
         <v>25</v>
       </c>
     </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27" s="7"/>
+      <c r="C27" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D27" s="7">
+        <v>5</v>
+      </c>
+      <c r="E27" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="F27" s="10"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="10"/>
+      <c r="I27" s="10"/>
+    </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D28" s="5"/>
+      <c r="A28" s="7"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="10"/>
+      <c r="H28" s="10"/>
+      <c r="I28" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="40">
-    <mergeCell ref="A21:B22"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="E21:I22"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="A7:B8"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="E11:I11"/>
-    <mergeCell ref="E12:I14"/>
-    <mergeCell ref="D12:D14"/>
-    <mergeCell ref="C12:C14"/>
-    <mergeCell ref="A12:B14"/>
-    <mergeCell ref="E9:I10"/>
-    <mergeCell ref="E7:I8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="A3:B4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="E4:I4"/>
-    <mergeCell ref="E5:I6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="A5:B6"/>
+  <mergeCells count="44">
+    <mergeCell ref="E27:I28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="A27:B28"/>
     <mergeCell ref="A26:B26"/>
     <mergeCell ref="A15:B15"/>
     <mergeCell ref="E15:I15"/>
@@ -878,6 +892,30 @@
     <mergeCell ref="D16:D18"/>
     <mergeCell ref="C16:C18"/>
     <mergeCell ref="E19:I20"/>
+    <mergeCell ref="A3:B4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="E4:I4"/>
+    <mergeCell ref="E5:I6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="A5:B6"/>
+    <mergeCell ref="A7:B8"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="E11:I11"/>
+    <mergeCell ref="E12:I14"/>
+    <mergeCell ref="D12:D14"/>
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="A12:B14"/>
+    <mergeCell ref="E9:I10"/>
+    <mergeCell ref="E7:I8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="A21:B22"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="E21:I22"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="C21:C22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Administracion de Costos y departamentos
</commit_message>
<xml_diff>
--- a/Horas de trabajo.xlsx
+++ b/Horas de trabajo.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="34">
   <si>
     <t>HOJA DE HORAS DE TRABAJO PROYECTO CENTROS DE COSTOS</t>
   </si>
@@ -111,6 +111,21 @@
   </si>
   <si>
     <t>Añadida funcionalidad para editar materiales y categorias. Los materiales mantienen su costo, el cual va a corresponder a su descripcion</t>
+  </si>
+  <si>
+    <t>16/7/2015</t>
+  </si>
+  <si>
+    <t>17/7/2015</t>
+  </si>
+  <si>
+    <t>Se comenzó con la sección de administrar costos y departamentos. Se agregaron las vistas para mostrar todos los costos, así como agregar nuevos y editarlos</t>
+  </si>
+  <si>
+    <t>Los costos y departamentos ya pueden ser administrados, se pueden crear y editar. Se expandió la entidad de departamentos para poder diferenciar departamentos que participen en el proceso productivo de los que no, y así poder mostrarlos en la sección de las fichas técnicas. También se le agregó una relación con los costos, para que cada departamento tenga sus costos asignados.</t>
+  </si>
+  <si>
+    <t>Total horas hasta ahora:</t>
   </si>
 </sst>
 </file>
@@ -169,20 +184,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -464,10 +479,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I28"/>
+  <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27:B28"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27:D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -515,34 +530,34 @@
       <c r="I4" s="7"/>
     </row>
     <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="6"/>
+      <c r="B5" s="8"/>
       <c r="C5" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D5" s="7">
         <v>4</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
-      <c r="B6" s="6"/>
+      <c r="A6" s="8"/>
+      <c r="B6" s="8"/>
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
@@ -555,57 +570,57 @@
       <c r="D7" s="7">
         <v>4</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E7" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="6">
+      <c r="A9" s="8">
         <v>42042</v>
       </c>
-      <c r="B9" s="6"/>
+      <c r="B9" s="8"/>
       <c r="C9" s="7" t="s">
         <v>12</v>
       </c>
       <c r="D9" s="7">
         <v>3</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="E9" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="6"/>
-      <c r="B10" s="6"/>
+      <c r="A10" s="8"/>
+      <c r="B10" s="8"/>
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="6">
+      <c r="A11" s="8">
         <v>42070</v>
       </c>
       <c r="B11" s="7"/>
@@ -624,48 +639,48 @@
       <c r="I11" s="9"/>
     </row>
     <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="6">
+      <c r="A12" s="8">
         <v>42101</v>
       </c>
-      <c r="B12" s="6"/>
+      <c r="B12" s="8"/>
       <c r="C12" s="7" t="s">
         <v>16</v>
       </c>
       <c r="D12" s="7">
         <v>8</v>
       </c>
-      <c r="E12" s="10" t="s">
+      <c r="E12" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="6"/>
-      <c r="B13" s="6"/>
+      <c r="A13" s="8"/>
+      <c r="B13" s="8"/>
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="6"/>
-      <c r="B14" s="6"/>
+      <c r="A14" s="8"/>
+      <c r="B14" s="8"/>
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="6">
+      <c r="A15" s="8">
         <v>42162</v>
       </c>
       <c r="B15" s="7"/>
@@ -684,146 +699,146 @@
       <c r="I15" s="9"/>
     </row>
     <row r="16" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="6">
+      <c r="A16" s="8">
         <v>42192</v>
       </c>
-      <c r="B16" s="6"/>
+      <c r="B16" s="8"/>
       <c r="C16" s="7" t="s">
         <v>10</v>
       </c>
       <c r="D16" s="7">
         <v>4</v>
       </c>
-      <c r="E16" s="8" t="s">
+      <c r="E16" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="6"/>
-      <c r="B17" s="6"/>
+      <c r="A17" s="8"/>
+      <c r="B17" s="8"/>
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
-      <c r="I17" s="8"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="6"/>
-      <c r="B18" s="6"/>
+      <c r="A18" s="8"/>
+      <c r="B18" s="8"/>
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="8"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="10"/>
     </row>
     <row r="19" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="6">
+      <c r="A19" s="8">
         <v>42284</v>
       </c>
-      <c r="B19" s="6"/>
+      <c r="B19" s="8"/>
       <c r="C19" s="7" t="s">
         <v>14</v>
       </c>
       <c r="D19" s="7">
         <v>4</v>
       </c>
-      <c r="E19" s="10" t="s">
+      <c r="E19" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="10"/>
-      <c r="I19" s="10"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="6"/>
-      <c r="B20" s="6"/>
+      <c r="A20" s="8"/>
+      <c r="B20" s="8"/>
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="10"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="10"/>
-      <c r="I20" s="10"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
     </row>
     <row r="21" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="6">
+      <c r="A21" s="8">
         <v>42315</v>
       </c>
-      <c r="B21" s="6"/>
+      <c r="B21" s="8"/>
       <c r="C21" s="7" t="s">
         <v>16</v>
       </c>
       <c r="D21" s="7">
         <v>4</v>
       </c>
-      <c r="E21" s="8" t="s">
+      <c r="E21" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="8"/>
-      <c r="I21" s="8"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="10"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="6"/>
-      <c r="B22" s="6"/>
+      <c r="A22" s="8"/>
+      <c r="B22" s="8"/>
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="8"/>
-      <c r="I22" s="8"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="10"/>
     </row>
     <row r="23" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="6">
+      <c r="A23" s="8">
         <v>42345</v>
       </c>
-      <c r="B23" s="6"/>
+      <c r="B23" s="8"/>
       <c r="C23" s="7" t="s">
         <v>23</v>
       </c>
       <c r="D23" s="7">
         <v>8</v>
       </c>
-      <c r="E23" s="8" t="s">
+      <c r="E23" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="F23" s="8"/>
-      <c r="G23" s="8"/>
-      <c r="H23" s="8"/>
-      <c r="I23" s="8"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="10"/>
+      <c r="I23" s="10"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="6"/>
-      <c r="B24" s="6"/>
+      <c r="A24" s="8"/>
+      <c r="B24" s="8"/>
       <c r="C24" s="7"/>
       <c r="D24" s="7"/>
-      <c r="E24" s="8"/>
-      <c r="F24" s="8"/>
-      <c r="G24" s="8"/>
-      <c r="H24" s="8"/>
-      <c r="I24" s="8"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="10"/>
+      <c r="I24" s="10"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="6"/>
-      <c r="B25" s="6"/>
+      <c r="A25" s="8"/>
+      <c r="B25" s="8"/>
       <c r="C25" s="7"/>
       <c r="D25" s="7"/>
-      <c r="E25" s="8"/>
-      <c r="F25" s="8"/>
-      <c r="G25" s="8"/>
-      <c r="H25" s="8"/>
-      <c r="I25" s="8"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="10"/>
+      <c r="I25" s="10"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
@@ -849,29 +864,124 @@
         <v>27</v>
       </c>
       <c r="D27" s="7">
-        <v>5</v>
-      </c>
-      <c r="E27" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E27" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="F27" s="10"/>
-      <c r="G27" s="10"/>
-      <c r="H27" s="10"/>
-      <c r="I27" s="10"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="6"/>
+      <c r="I27" s="6"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="7"/>
       <c r="B28" s="7"/>
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
-      <c r="E28" s="10"/>
-      <c r="F28" s="10"/>
-      <c r="G28" s="10"/>
-      <c r="H28" s="10"/>
-      <c r="I28" s="10"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="6"/>
+      <c r="I28" s="6"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29" s="7"/>
+      <c r="C29" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D29" s="7">
+        <v>4</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="6"/>
+      <c r="I29" s="6"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="7"/>
+      <c r="B30" s="7"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="6"/>
+      <c r="I30" s="6"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B31" s="7"/>
+      <c r="C31" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D31" s="7">
+        <v>8</v>
+      </c>
+      <c r="E31" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="F31" s="10"/>
+      <c r="G31" s="10"/>
+      <c r="H31" s="10"/>
+      <c r="I31" s="10"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="7"/>
+      <c r="B32" s="7"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="10"/>
+      <c r="F32" s="10"/>
+      <c r="G32" s="10"/>
+      <c r="H32" s="10"/>
+      <c r="I32" s="10"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="7"/>
+      <c r="B33" s="7"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="10"/>
+      <c r="F33" s="10"/>
+      <c r="G33" s="10"/>
+      <c r="H33" s="10"/>
+      <c r="I33" s="10"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="7"/>
+      <c r="B34" s="7"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="10"/>
+      <c r="F34" s="10"/>
+      <c r="G34" s="10"/>
+      <c r="H34" s="10"/>
+      <c r="I34" s="10"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>33</v>
+      </c>
+      <c r="D41">
+        <f>SUM(D5:D40)</f>
+        <v>66</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="44">
+  <mergeCells count="52">
+    <mergeCell ref="E31:I34"/>
+    <mergeCell ref="D31:D34"/>
+    <mergeCell ref="C31:C34"/>
+    <mergeCell ref="A31:B34"/>
     <mergeCell ref="E27:I28"/>
     <mergeCell ref="D27:D28"/>
     <mergeCell ref="C27:C28"/>
@@ -882,7 +992,6 @@
     <mergeCell ref="A9:B10"/>
     <mergeCell ref="C9:C10"/>
     <mergeCell ref="D9:D10"/>
-    <mergeCell ref="A19:B20"/>
     <mergeCell ref="A16:B18"/>
     <mergeCell ref="E23:I25"/>
     <mergeCell ref="D23:D25"/>
@@ -892,6 +1001,12 @@
     <mergeCell ref="D16:D18"/>
     <mergeCell ref="C16:C18"/>
     <mergeCell ref="E19:I20"/>
+    <mergeCell ref="A21:B22"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="E21:I22"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="C21:C22"/>
     <mergeCell ref="A3:B4"/>
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="E4:I4"/>
@@ -899,6 +1014,10 @@
     <mergeCell ref="D5:D6"/>
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="A5:B6"/>
+    <mergeCell ref="E29:I30"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="A29:B30"/>
     <mergeCell ref="A7:B8"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="E11:I11"/>
@@ -910,12 +1029,7 @@
     <mergeCell ref="E7:I8"/>
     <mergeCell ref="D7:D8"/>
     <mergeCell ref="C7:C8"/>
-    <mergeCell ref="A21:B22"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="E21:I22"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="A19:B20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Se reestructuro el modelo materiales
Se elimino el campo costos de ellos
</commit_message>
<xml_diff>
--- a/Horas de trabajo.xlsx
+++ b/Horas de trabajo.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="76">
   <si>
     <t>HOJA DE HORAS DE TRABAJO PROYECTO CENTROS DE COSTOS</t>
   </si>
@@ -171,6 +171,87 @@
   </si>
   <si>
     <t>Se agregaron usuarios de prueba para poder autenticarse a la aplicación, y también se crearon nuevas migraciones en la base de datos</t>
+  </si>
+  <si>
+    <t>22/9/2015</t>
+  </si>
+  <si>
+    <t>Se agregó la vista para autenticacción, además del botón para cerrar la sesión</t>
+  </si>
+  <si>
+    <t>25/9/2015</t>
+  </si>
+  <si>
+    <t>Se corrigieron errores en las vistas, el usuario no se autenticaba correctamente en algunas ocaciones</t>
+  </si>
+  <si>
+    <t>26/9/2015</t>
+  </si>
+  <si>
+    <t>Se agregó la opción para poder seleccionar el departamento al cual corresponden los materiales, además, el costo generado al crear ese material puede modificarse de la misma manera</t>
+  </si>
+  <si>
+    <t>Horas totales</t>
+  </si>
+  <si>
+    <t>Horas pagadas</t>
+  </si>
+  <si>
+    <t>Horas pendientes</t>
+  </si>
+  <si>
+    <t>Se reestructuró el código para que los controladores se vean más ordenados y se pueda trabajar más fácil en ellos, también se agrego la funcionalidad para importar lineas y modelos desde excel</t>
+  </si>
+  <si>
+    <t>Las lineas ahora pueden importarse desde excel, la vista tambien permite importar los modelos de todas las lineas desde un solo archivo, o también agregar los modelos linea por linea</t>
+  </si>
+  <si>
+    <t>15/10/2015</t>
+  </si>
+  <si>
+    <t>16/10/2015</t>
+  </si>
+  <si>
+    <t>Se arregló un bug a la hora de importar las lineas que estaba causando que la base de datos se borrara</t>
+  </si>
+  <si>
+    <t>Se creó la funcionalidad para mostrar las fichas técnicas de los modelos de zapato</t>
+  </si>
+  <si>
+    <t>Se puede ingresar a una linea e importar los modelos para esa linea en especifico</t>
+  </si>
+  <si>
+    <t>23/10/2015</t>
+  </si>
+  <si>
+    <t>Se puede importar los materiales desde la hoja de excel, se necesita tener creada la categoria anteriormente, además genera el costo automáticamente</t>
+  </si>
+  <si>
+    <t>Para mejorar la administracion de los materiales, fueron divididos por páginas para que se pueda navegar por ellos fácilmente</t>
+  </si>
+  <si>
+    <t>Se pueden buscar materiales a través de un textbox, la busqueda queda filtrada luego de cambiar la página</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reunión en MEMBO para conocer los detalles sobre la hoja de costos. </t>
+  </si>
+  <si>
+    <t>13/11/2015</t>
+  </si>
+  <si>
+    <t>15/11/2015</t>
+  </si>
+  <si>
+    <t>Reestructurado el código que permite subir la imagen del modelo, ahora la imagen se genera con un id único y no generará problemas a la hora de subir otras imágenes. Además, se mejoró el diseño de las fichas técnicas para mostrar mejor la información</t>
+  </si>
+  <si>
+    <t>Reestructurado el código inicial de las fichas técnicas, debido a que era muy dificil de entender</t>
+  </si>
+  <si>
+    <t>21/11/2015</t>
+  </si>
+  <si>
+    <t>Se hizo una reestructuración al modelo de datos, haciendo que los materiales no generen un costo al ser agregados, de esta manera, los materiales serán directamente agregados a la ficha técnica. El costo será calculado a partir de un total de los valores de estos materiales, y se asignará al costo que pertenece a materia prima directa o indireta. Se presentó un problema con la base de datos, generó una lista de bugs inesperados y se tuvo que regenerar el código desde el repositorio en linea para poder seguir trabajando.</t>
   </si>
 </sst>
 </file>
@@ -194,7 +275,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -204,6 +285,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -220,7 +319,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -245,15 +344,64 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -261,12 +409,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -548,15 +690,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I44"/>
+  <dimension ref="A1:M69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44:B44"/>
+    <sheetView tabSelected="1" topLeftCell="A50" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E62" sqref="E62:I64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="75" customWidth="1"/>
   </cols>
@@ -572,348 +715,348 @@
       <c r="G1" s="1"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="10"/>
+      <c r="B3" s="18"/>
       <c r="C3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="18" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="10"/>
-      <c r="B4" s="10"/>
+      <c r="A4" s="18"/>
+      <c r="B4" s="18"/>
       <c r="C4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10" t="s">
+      <c r="D4" s="18"/>
+      <c r="E4" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="18"/>
     </row>
     <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="12"/>
-      <c r="C5" s="10" t="s">
+      <c r="B5" s="21"/>
+      <c r="C5" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="10">
-        <v>4</v>
-      </c>
-      <c r="E5" s="15" t="s">
+      <c r="D5" s="18">
+        <v>4</v>
+      </c>
+      <c r="E5" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="19"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="12"/>
-      <c r="B6" s="12"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="15"/>
+      <c r="A6" s="21"/>
+      <c r="B6" s="21"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10" t="s">
+      <c r="B7" s="18"/>
+      <c r="C7" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="10">
-        <v>4</v>
-      </c>
-      <c r="E7" s="15" t="s">
+      <c r="D7" s="18">
+        <v>4</v>
+      </c>
+      <c r="E7" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="15"/>
-      <c r="I7" s="15"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="10"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
+      <c r="A8" s="18"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="19"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="12">
+      <c r="A9" s="21">
         <v>42042</v>
       </c>
-      <c r="B9" s="12"/>
-      <c r="C9" s="10" t="s">
+      <c r="B9" s="21"/>
+      <c r="C9" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="10">
+      <c r="D9" s="18">
         <v>3</v>
       </c>
-      <c r="E9" s="15" t="s">
+      <c r="E9" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="15"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="19"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="12"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="15"/>
+      <c r="A10" s="21"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="19"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="12">
+      <c r="A11" s="21">
         <v>42070</v>
       </c>
-      <c r="B11" s="10"/>
+      <c r="B11" s="18"/>
       <c r="C11" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D11" s="3">
         <v>3</v>
       </c>
-      <c r="E11" s="16" t="s">
+      <c r="E11" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="16"/>
-      <c r="G11" s="16"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="16"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="28"/>
+      <c r="I11" s="28"/>
     </row>
     <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="12">
+      <c r="A12" s="21">
         <v>42101</v>
       </c>
-      <c r="B12" s="12"/>
-      <c r="C12" s="10" t="s">
+      <c r="B12" s="21"/>
+      <c r="C12" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="10">
+      <c r="D12" s="18">
         <v>8</v>
       </c>
-      <c r="E12" s="15" t="s">
+      <c r="E12" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="F12" s="15"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="15"/>
-      <c r="I12" s="15"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="19"/>
+      <c r="H12" s="19"/>
+      <c r="I12" s="19"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="12"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="15"/>
-      <c r="I13" s="15"/>
+      <c r="A13" s="21"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="19"/>
+      <c r="I13" s="19"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="12"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="15"/>
-      <c r="I14" s="15"/>
+      <c r="A14" s="21"/>
+      <c r="B14" s="21"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="19"/>
+      <c r="H14" s="19"/>
+      <c r="I14" s="19"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="12">
+      <c r="A15" s="21">
         <v>42162</v>
       </c>
-      <c r="B15" s="10"/>
+      <c r="B15" s="18"/>
       <c r="C15" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D15" s="4">
         <v>4</v>
       </c>
-      <c r="E15" s="16" t="s">
+      <c r="E15" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="F15" s="16"/>
-      <c r="G15" s="16"/>
-      <c r="H15" s="16"/>
-      <c r="I15" s="16"/>
+      <c r="F15" s="28"/>
+      <c r="G15" s="28"/>
+      <c r="H15" s="28"/>
+      <c r="I15" s="28"/>
     </row>
     <row r="16" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="11">
+      <c r="A16" s="29">
         <v>42192</v>
       </c>
-      <c r="B16" s="11"/>
-      <c r="C16" s="14" t="s">
+      <c r="B16" s="29"/>
+      <c r="C16" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="D16" s="14">
-        <v>4</v>
-      </c>
-      <c r="E16" s="13" t="s">
+      <c r="D16" s="31">
+        <v>4</v>
+      </c>
+      <c r="E16" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="13"/>
-      <c r="I16" s="13"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="30"/>
+      <c r="H16" s="30"/>
+      <c r="I16" s="30"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="11"/>
-      <c r="B17" s="11"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="13"/>
-      <c r="I17" s="13"/>
+      <c r="A17" s="29"/>
+      <c r="B17" s="29"/>
+      <c r="C17" s="31"/>
+      <c r="D17" s="31"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="30"/>
+      <c r="G17" s="30"/>
+      <c r="H17" s="30"/>
+      <c r="I17" s="30"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="11"/>
-      <c r="B18" s="11"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="13"/>
-      <c r="I18" s="13"/>
+      <c r="A18" s="29"/>
+      <c r="B18" s="29"/>
+      <c r="C18" s="31"/>
+      <c r="D18" s="31"/>
+      <c r="E18" s="30"/>
+      <c r="F18" s="30"/>
+      <c r="G18" s="30"/>
+      <c r="H18" s="30"/>
+      <c r="I18" s="30"/>
     </row>
     <row r="19" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="12">
+      <c r="A19" s="21">
         <v>42284</v>
       </c>
-      <c r="B19" s="12"/>
-      <c r="C19" s="10" t="s">
+      <c r="B19" s="21"/>
+      <c r="C19" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="D19" s="10">
-        <v>4</v>
-      </c>
-      <c r="E19" s="15" t="s">
+      <c r="D19" s="18">
+        <v>4</v>
+      </c>
+      <c r="E19" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="F19" s="15"/>
-      <c r="G19" s="15"/>
-      <c r="H19" s="15"/>
-      <c r="I19" s="15"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="19"/>
+      <c r="H19" s="19"/>
+      <c r="I19" s="19"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="12"/>
-      <c r="B20" s="12"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="15"/>
-      <c r="F20" s="15"/>
-      <c r="G20" s="15"/>
-      <c r="H20" s="15"/>
-      <c r="I20" s="15"/>
+      <c r="A20" s="21"/>
+      <c r="B20" s="21"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="19"/>
+      <c r="H20" s="19"/>
+      <c r="I20" s="19"/>
     </row>
     <row r="21" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="12">
+      <c r="A21" s="21">
         <v>42315</v>
       </c>
-      <c r="B21" s="12"/>
-      <c r="C21" s="10" t="s">
+      <c r="B21" s="21"/>
+      <c r="C21" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="D21" s="10">
-        <v>4</v>
-      </c>
-      <c r="E21" s="9" t="s">
+      <c r="D21" s="18">
+        <v>4</v>
+      </c>
+      <c r="E21" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
-      <c r="H21" s="9"/>
-      <c r="I21" s="9"/>
+      <c r="F21" s="27"/>
+      <c r="G21" s="27"/>
+      <c r="H21" s="27"/>
+      <c r="I21" s="27"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="12"/>
-      <c r="B22" s="12"/>
-      <c r="C22" s="10"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
-      <c r="G22" s="9"/>
-      <c r="H22" s="9"/>
-      <c r="I22" s="9"/>
+      <c r="A22" s="21"/>
+      <c r="B22" s="21"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="27"/>
+      <c r="F22" s="27"/>
+      <c r="G22" s="27"/>
+      <c r="H22" s="27"/>
+      <c r="I22" s="27"/>
     </row>
     <row r="23" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="12">
+      <c r="A23" s="21">
         <v>42345</v>
       </c>
-      <c r="B23" s="12"/>
-      <c r="C23" s="10" t="s">
+      <c r="B23" s="21"/>
+      <c r="C23" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="D23" s="10">
+      <c r="D23" s="18">
         <v>8</v>
       </c>
-      <c r="E23" s="9" t="s">
+      <c r="E23" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="F23" s="9"/>
-      <c r="G23" s="9"/>
-      <c r="H23" s="9"/>
-      <c r="I23" s="9"/>
+      <c r="F23" s="27"/>
+      <c r="G23" s="27"/>
+      <c r="H23" s="27"/>
+      <c r="I23" s="27"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="12"/>
-      <c r="B24" s="12"/>
-      <c r="C24" s="10"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="9"/>
-      <c r="G24" s="9"/>
-      <c r="H24" s="9"/>
-      <c r="I24" s="9"/>
+      <c r="A24" s="21"/>
+      <c r="B24" s="21"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="27"/>
+      <c r="F24" s="27"/>
+      <c r="G24" s="27"/>
+      <c r="H24" s="27"/>
+      <c r="I24" s="27"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="12"/>
-      <c r="B25" s="12"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="9"/>
-      <c r="F25" s="9"/>
-      <c r="G25" s="9"/>
-      <c r="H25" s="9"/>
-      <c r="I25" s="9"/>
+      <c r="A25" s="21"/>
+      <c r="B25" s="21"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="27"/>
+      <c r="F25" s="27"/>
+      <c r="G25" s="27"/>
+      <c r="H25" s="27"/>
+      <c r="I25" s="27"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="10" t="s">
+      <c r="A26" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="10"/>
+      <c r="B26" s="18"/>
       <c r="C26" s="5" t="s">
         <v>6</v>
       </c>
@@ -925,122 +1068,122 @@
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="10" t="s">
+      <c r="A27" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="10"/>
-      <c r="C27" s="10" t="s">
+      <c r="B27" s="18"/>
+      <c r="C27" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="D27" s="10">
-        <v>4</v>
-      </c>
-      <c r="E27" s="15" t="s">
+      <c r="D27" s="18">
+        <v>4</v>
+      </c>
+      <c r="E27" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="F27" s="15"/>
-      <c r="G27" s="15"/>
-      <c r="H27" s="15"/>
-      <c r="I27" s="15"/>
+      <c r="F27" s="19"/>
+      <c r="G27" s="19"/>
+      <c r="H27" s="19"/>
+      <c r="I27" s="19"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="10"/>
-      <c r="B28" s="10"/>
-      <c r="C28" s="10"/>
-      <c r="D28" s="10"/>
-      <c r="E28" s="15"/>
-      <c r="F28" s="15"/>
-      <c r="G28" s="15"/>
-      <c r="H28" s="15"/>
-      <c r="I28" s="15"/>
+      <c r="A28" s="18"/>
+      <c r="B28" s="18"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="19"/>
+      <c r="I28" s="19"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="10" t="s">
+      <c r="A29" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="B29" s="10"/>
-      <c r="C29" s="10" t="s">
+      <c r="B29" s="18"/>
+      <c r="C29" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="D29" s="10">
-        <v>4</v>
-      </c>
-      <c r="E29" s="15" t="s">
+      <c r="D29" s="18">
+        <v>4</v>
+      </c>
+      <c r="E29" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="F29" s="15"/>
-      <c r="G29" s="15"/>
-      <c r="H29" s="15"/>
-      <c r="I29" s="15"/>
+      <c r="F29" s="19"/>
+      <c r="G29" s="19"/>
+      <c r="H29" s="19"/>
+      <c r="I29" s="19"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="10"/>
-      <c r="B30" s="10"/>
-      <c r="C30" s="10"/>
-      <c r="D30" s="10"/>
-      <c r="E30" s="15"/>
-      <c r="F30" s="15"/>
-      <c r="G30" s="15"/>
-      <c r="H30" s="15"/>
-      <c r="I30" s="15"/>
+      <c r="A30" s="18"/>
+      <c r="B30" s="18"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="19"/>
+      <c r="F30" s="19"/>
+      <c r="G30" s="19"/>
+      <c r="H30" s="19"/>
+      <c r="I30" s="19"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="10" t="s">
+      <c r="A31" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="B31" s="10"/>
-      <c r="C31" s="10" t="s">
+      <c r="B31" s="18"/>
+      <c r="C31" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="D31" s="10">
+      <c r="D31" s="18">
         <v>8</v>
       </c>
-      <c r="E31" s="9" t="s">
+      <c r="E31" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="F31" s="9"/>
-      <c r="G31" s="9"/>
-      <c r="H31" s="9"/>
-      <c r="I31" s="9"/>
+      <c r="F31" s="27"/>
+      <c r="G31" s="27"/>
+      <c r="H31" s="27"/>
+      <c r="I31" s="27"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="10"/>
-      <c r="B32" s="10"/>
-      <c r="C32" s="10"/>
-      <c r="D32" s="10"/>
-      <c r="E32" s="9"/>
-      <c r="F32" s="9"/>
-      <c r="G32" s="9"/>
-      <c r="H32" s="9"/>
-      <c r="I32" s="9"/>
+      <c r="A32" s="18"/>
+      <c r="B32" s="18"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="27"/>
+      <c r="F32" s="27"/>
+      <c r="G32" s="27"/>
+      <c r="H32" s="27"/>
+      <c r="I32" s="27"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="10"/>
-      <c r="B33" s="10"/>
-      <c r="C33" s="10"/>
-      <c r="D33" s="10"/>
-      <c r="E33" s="9"/>
-      <c r="F33" s="9"/>
-      <c r="G33" s="9"/>
-      <c r="H33" s="9"/>
-      <c r="I33" s="9"/>
+      <c r="A33" s="18"/>
+      <c r="B33" s="18"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="27"/>
+      <c r="F33" s="27"/>
+      <c r="G33" s="27"/>
+      <c r="H33" s="27"/>
+      <c r="I33" s="27"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="10"/>
-      <c r="B34" s="10"/>
-      <c r="C34" s="10"/>
-      <c r="D34" s="10"/>
-      <c r="E34" s="9"/>
-      <c r="F34" s="9"/>
-      <c r="G34" s="9"/>
-      <c r="H34" s="9"/>
-      <c r="I34" s="9"/>
+      <c r="A34" s="18"/>
+      <c r="B34" s="18"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="27"/>
+      <c r="F34" s="27"/>
+      <c r="G34" s="27"/>
+      <c r="H34" s="27"/>
+      <c r="I34" s="27"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="10" t="s">
+      <c r="A35" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="B35" s="10"/>
+      <c r="B35" s="18"/>
       <c r="C35" s="6" t="s">
         <v>16</v>
       </c>
@@ -1052,40 +1195,40 @@
       </c>
     </row>
     <row r="36" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="10" t="s">
+      <c r="A36" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="B36" s="10"/>
-      <c r="C36" s="10" t="s">
+      <c r="B36" s="18"/>
+      <c r="C36" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="D36" s="10">
+      <c r="D36" s="18">
         <v>8</v>
       </c>
-      <c r="E36" s="9" t="s">
+      <c r="E36" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="F36" s="9"/>
-      <c r="G36" s="9"/>
-      <c r="H36" s="9"/>
-      <c r="I36" s="9"/>
+      <c r="F36" s="27"/>
+      <c r="G36" s="27"/>
+      <c r="H36" s="27"/>
+      <c r="I36" s="27"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="10"/>
-      <c r="B37" s="10"/>
-      <c r="C37" s="10"/>
-      <c r="D37" s="10"/>
-      <c r="E37" s="9"/>
-      <c r="F37" s="9"/>
-      <c r="G37" s="9"/>
-      <c r="H37" s="9"/>
-      <c r="I37" s="9"/>
+      <c r="A37" s="18"/>
+      <c r="B37" s="18"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="27"/>
+      <c r="F37" s="27"/>
+      <c r="G37" s="27"/>
+      <c r="H37" s="27"/>
+      <c r="I37" s="27"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="10" t="s">
+      <c r="A38" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="B38" s="10"/>
+      <c r="B38" s="18"/>
       <c r="C38" s="7" t="s">
         <v>6</v>
       </c>
@@ -1097,40 +1240,40 @@
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="10" t="s">
+      <c r="A39" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="B39" s="10"/>
-      <c r="C39" s="10" t="s">
+      <c r="B39" s="18"/>
+      <c r="C39" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="D39" s="10">
-        <v>4</v>
-      </c>
-      <c r="E39" s="9" t="s">
+      <c r="D39" s="18">
+        <v>4</v>
+      </c>
+      <c r="E39" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="F39" s="9"/>
-      <c r="G39" s="9"/>
-      <c r="H39" s="9"/>
-      <c r="I39" s="9"/>
+      <c r="F39" s="27"/>
+      <c r="G39" s="27"/>
+      <c r="H39" s="27"/>
+      <c r="I39" s="27"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="10"/>
-      <c r="B40" s="10"/>
-      <c r="C40" s="10"/>
-      <c r="D40" s="10"/>
-      <c r="E40" s="9"/>
-      <c r="F40" s="9"/>
-      <c r="G40" s="9"/>
-      <c r="H40" s="9"/>
-      <c r="I40" s="9"/>
+      <c r="A40" s="18"/>
+      <c r="B40" s="18"/>
+      <c r="C40" s="18"/>
+      <c r="D40" s="18"/>
+      <c r="E40" s="27"/>
+      <c r="F40" s="27"/>
+      <c r="G40" s="27"/>
+      <c r="H40" s="27"/>
+      <c r="I40" s="27"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="10" t="s">
+      <c r="A41" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="B41" s="10"/>
+      <c r="B41" s="18"/>
       <c r="C41" s="8" t="s">
         <v>6</v>
       </c>
@@ -1142,10 +1285,10 @@
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="10" t="s">
+      <c r="A42" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="B42" s="10"/>
+      <c r="B42" s="18"/>
       <c r="C42" s="8" t="s">
         <v>10</v>
       </c>
@@ -1157,10 +1300,10 @@
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" s="10" t="s">
+      <c r="A43" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="B43" s="10"/>
+      <c r="B43" s="18"/>
       <c r="C43" s="8" t="s">
         <v>14</v>
       </c>
@@ -1172,10 +1315,10 @@
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="10" t="s">
+      <c r="A44" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="B44" s="10"/>
+      <c r="B44" s="18"/>
       <c r="C44" s="8" t="s">
         <v>16</v>
       </c>
@@ -1186,47 +1329,426 @@
         <v>48</v>
       </c>
     </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="B45" s="18"/>
+      <c r="C45" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D45" s="9">
+        <v>3</v>
+      </c>
+      <c r="E45" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="B46" s="26"/>
+      <c r="C46" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D46" s="12">
+        <v>2</v>
+      </c>
+      <c r="E46" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="F46" s="13"/>
+      <c r="G46" s="13"/>
+      <c r="H46" s="13"/>
+      <c r="I46" s="13"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="B47" s="25"/>
+      <c r="C47" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D47" s="25">
+        <v>4</v>
+      </c>
+      <c r="E47" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="F47" s="24"/>
+      <c r="G47" s="24"/>
+      <c r="H47" s="24"/>
+      <c r="I47" s="24"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" s="25"/>
+      <c r="B48" s="25"/>
+      <c r="C48" s="25"/>
+      <c r="D48" s="25"/>
+      <c r="E48" s="24"/>
+      <c r="F48" s="24"/>
+      <c r="G48" s="24"/>
+      <c r="H48" s="24"/>
+      <c r="I48" s="24"/>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A49" s="21">
+        <v>42134</v>
+      </c>
+      <c r="B49" s="21"/>
+      <c r="C49" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D49" s="20">
+        <v>4</v>
+      </c>
+      <c r="E49" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="F49" s="19"/>
+      <c r="G49" s="19"/>
+      <c r="H49" s="19"/>
+      <c r="I49" s="19"/>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A50" s="21"/>
+      <c r="B50" s="21"/>
+      <c r="C50" s="20"/>
+      <c r="D50" s="20"/>
+      <c r="E50" s="19"/>
+      <c r="F50" s="19"/>
+      <c r="G50" s="19"/>
+      <c r="H50" s="19"/>
+      <c r="I50" s="19"/>
+      <c r="L50" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="M50" s="23"/>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A51" s="21">
+        <v>42165</v>
+      </c>
+      <c r="B51" s="21"/>
+      <c r="C51" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="D51" s="20">
+        <v>8</v>
+      </c>
+      <c r="E51" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="F51" s="19"/>
+      <c r="G51" s="19"/>
+      <c r="H51" s="19"/>
+      <c r="I51" s="19"/>
+      <c r="L51" s="22">
+        <f>SUM(D5:D69)</f>
+        <v>183</v>
+      </c>
+      <c r="M51" s="22"/>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A52" s="21"/>
+      <c r="B52" s="21"/>
+      <c r="C52" s="20"/>
+      <c r="D52" s="20"/>
+      <c r="E52" s="19"/>
+      <c r="F52" s="19"/>
+      <c r="G52" s="19"/>
+      <c r="H52" s="19"/>
+      <c r="I52" s="19"/>
+      <c r="L52" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="M52" s="23"/>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A53" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="B53" s="18"/>
+      <c r="C53" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D53" s="10">
+        <v>4</v>
+      </c>
+      <c r="E53" t="s">
+        <v>62</v>
+      </c>
+      <c r="L53" s="22">
+        <f>SUM(D5:D48)</f>
+        <v>119</v>
+      </c>
+      <c r="M53" s="22"/>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A54" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="B54" s="18"/>
+      <c r="C54" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D54" s="10">
+        <v>8</v>
+      </c>
+      <c r="E54" t="s">
+        <v>63</v>
+      </c>
+      <c r="L54" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="M54" s="23"/>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A55" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="B55" s="18"/>
+      <c r="C55" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D55" s="11">
+        <v>4</v>
+      </c>
+      <c r="E55" t="s">
+        <v>64</v>
+      </c>
+      <c r="L55" s="22">
+        <f>SUM(D49:D69)</f>
+        <v>64</v>
+      </c>
+      <c r="M55" s="22"/>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A56" s="21">
+        <v>42166</v>
+      </c>
+      <c r="B56" s="21"/>
+      <c r="C56" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D56" s="20">
+        <v>8</v>
+      </c>
+      <c r="E56" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="F56" s="19"/>
+      <c r="G56" s="19"/>
+      <c r="H56" s="19"/>
+      <c r="I56" s="19"/>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A57" s="21"/>
+      <c r="B57" s="21"/>
+      <c r="C57" s="20"/>
+      <c r="D57" s="20"/>
+      <c r="E57" s="19"/>
+      <c r="F57" s="19"/>
+      <c r="G57" s="19"/>
+      <c r="H57" s="19"/>
+      <c r="I57" s="19"/>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A58" s="21">
+        <v>42196</v>
+      </c>
+      <c r="B58" s="21"/>
+      <c r="C58" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D58" s="14">
+        <v>4</v>
+      </c>
+      <c r="E58" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A59" s="21">
+        <v>42227</v>
+      </c>
+      <c r="B59" s="21"/>
+      <c r="C59" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="D59" s="15">
+        <v>4</v>
+      </c>
+      <c r="E59" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A60" s="21">
+        <v>42288</v>
+      </c>
+      <c r="B60" s="21"/>
+      <c r="C60" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="D60" s="16">
+        <v>4</v>
+      </c>
+      <c r="E60" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A61" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="B61" s="18"/>
+      <c r="C61" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D61" s="17">
+        <v>2</v>
+      </c>
+      <c r="E61" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="B62" s="18"/>
+      <c r="C62" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="D62" s="20">
+        <v>6</v>
+      </c>
+      <c r="E62" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="F62" s="19"/>
+      <c r="G62" s="19"/>
+      <c r="H62" s="19"/>
+      <c r="I62" s="19"/>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A63" s="18"/>
+      <c r="B63" s="18"/>
+      <c r="C63" s="20"/>
+      <c r="D63" s="20"/>
+      <c r="E63" s="19"/>
+      <c r="F63" s="19"/>
+      <c r="G63" s="19"/>
+      <c r="H63" s="19"/>
+      <c r="I63" s="19"/>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A64" s="18"/>
+      <c r="B64" s="18"/>
+      <c r="C64" s="20"/>
+      <c r="D64" s="20"/>
+      <c r="E64" s="19"/>
+      <c r="F64" s="19"/>
+      <c r="G64" s="19"/>
+      <c r="H64" s="19"/>
+      <c r="I64" s="19"/>
+    </row>
+    <row r="65" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="B65" s="18"/>
+      <c r="C65" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="D65" s="20">
+        <v>8</v>
+      </c>
+      <c r="E65" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="F65" s="19"/>
+      <c r="G65" s="19"/>
+      <c r="H65" s="19"/>
+      <c r="I65" s="19"/>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A66" s="18"/>
+      <c r="B66" s="18"/>
+      <c r="C66" s="20"/>
+      <c r="D66" s="20"/>
+      <c r="E66" s="19"/>
+      <c r="F66" s="19"/>
+      <c r="G66" s="19"/>
+      <c r="H66" s="19"/>
+      <c r="I66" s="19"/>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A67" s="18"/>
+      <c r="B67" s="18"/>
+      <c r="C67" s="20"/>
+      <c r="D67" s="20"/>
+      <c r="E67" s="19"/>
+      <c r="F67" s="19"/>
+      <c r="G67" s="19"/>
+      <c r="H67" s="19"/>
+      <c r="I67" s="19"/>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A68" s="18"/>
+      <c r="B68" s="18"/>
+      <c r="C68" s="20"/>
+      <c r="D68" s="20"/>
+      <c r="E68" s="19"/>
+      <c r="F68" s="19"/>
+      <c r="G68" s="19"/>
+      <c r="H68" s="19"/>
+      <c r="I68" s="19"/>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A69" s="18"/>
+      <c r="B69" s="18"/>
+      <c r="C69" s="20"/>
+      <c r="D69" s="20"/>
+      <c r="E69" s="19"/>
+      <c r="F69" s="19"/>
+      <c r="G69" s="19"/>
+      <c r="H69" s="19"/>
+      <c r="I69" s="19"/>
+    </row>
   </sheetData>
-  <mergeCells count="66">
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="A26:B26"/>
+  <mergeCells count="105">
+    <mergeCell ref="E65:I69"/>
+    <mergeCell ref="D65:D69"/>
+    <mergeCell ref="C65:C69"/>
+    <mergeCell ref="A65:B69"/>
+    <mergeCell ref="E62:I64"/>
+    <mergeCell ref="D62:D64"/>
+    <mergeCell ref="C62:C64"/>
+    <mergeCell ref="A62:B64"/>
+    <mergeCell ref="E29:I30"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="E39:I40"/>
+    <mergeCell ref="A29:B30"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A36:B37"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="C39:C40"/>
     <mergeCell ref="E31:I34"/>
     <mergeCell ref="D31:D34"/>
     <mergeCell ref="C31:C34"/>
     <mergeCell ref="A31:B34"/>
-    <mergeCell ref="E27:I28"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="A27:B28"/>
-    <mergeCell ref="E29:I30"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="A7:B8"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="E11:I11"/>
-    <mergeCell ref="E12:I14"/>
-    <mergeCell ref="D12:D14"/>
-    <mergeCell ref="C12:C14"/>
-    <mergeCell ref="A12:B14"/>
-    <mergeCell ref="E9:I10"/>
-    <mergeCell ref="E7:I8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="A3:B4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="E4:I4"/>
-    <mergeCell ref="E5:I6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="A5:B6"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="E15:I15"/>
-    <mergeCell ref="A9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="A51:B52"/>
+    <mergeCell ref="A49:B50"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="A59:B59"/>
     <mergeCell ref="A16:B18"/>
     <mergeCell ref="E23:I25"/>
     <mergeCell ref="D23:D25"/>
@@ -1242,18 +1764,68 @@
     <mergeCell ref="C19:C20"/>
     <mergeCell ref="E21:I22"/>
     <mergeCell ref="D21:D22"/>
+    <mergeCell ref="E7:I8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="E15:I15"/>
+    <mergeCell ref="A3:B4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="E4:I4"/>
+    <mergeCell ref="E5:I6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="A5:B6"/>
+    <mergeCell ref="A9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="A7:B8"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="E11:I11"/>
+    <mergeCell ref="E12:I14"/>
+    <mergeCell ref="D12:D14"/>
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="A12:B14"/>
+    <mergeCell ref="E9:I10"/>
     <mergeCell ref="C21:C22"/>
-    <mergeCell ref="E39:I40"/>
-    <mergeCell ref="A29:B30"/>
-    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="E47:I48"/>
+    <mergeCell ref="D47:D48"/>
+    <mergeCell ref="C47:C48"/>
+    <mergeCell ref="A47:B48"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="A44:B44"/>
     <mergeCell ref="E36:I37"/>
     <mergeCell ref="D36:D37"/>
     <mergeCell ref="C36:C37"/>
-    <mergeCell ref="A36:B37"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="C39:C40"/>
     <mergeCell ref="A39:B40"/>
     <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="E27:I28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="A27:B28"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="E56:I57"/>
+    <mergeCell ref="D56:D57"/>
+    <mergeCell ref="C56:C57"/>
+    <mergeCell ref="A56:B57"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="L55:M55"/>
+    <mergeCell ref="L50:M50"/>
+    <mergeCell ref="L51:M51"/>
+    <mergeCell ref="L52:M52"/>
+    <mergeCell ref="L53:M53"/>
+    <mergeCell ref="L54:M54"/>
+    <mergeCell ref="E51:I52"/>
+    <mergeCell ref="D51:D52"/>
+    <mergeCell ref="C51:C52"/>
+    <mergeCell ref="E49:I50"/>
+    <mergeCell ref="D49:D50"/>
+    <mergeCell ref="C49:C50"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Calculo de costos directos e indirectos
</commit_message>
<xml_diff>
--- a/Horas de trabajo.xlsx
+++ b/Horas de trabajo.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="89">
   <si>
     <t>HOJA DE HORAS DE TRABAJO PROYECTO CENTROS DE COSTOS</t>
   </si>
@@ -251,7 +251,46 @@
     <t>21/11/2015</t>
   </si>
   <si>
-    <t>Se hizo una reestructuración al modelo de datos, haciendo que los materiales no generen un costo al ser agregados, de esta manera, los materiales serán directamente agregados a la ficha técnica. El costo será calculado a partir de un total de los valores de estos materiales, y se asignará al costo que pertenece a materia prima directa o indireta. Se presentó un problema con la base de datos, generó una lista de bugs inesperados y se tuvo que regenerar el código desde el repositorio en linea para poder seguir trabajando.</t>
+    <t>Se hizo una reestructuración al modelo de datos, haciendo que los materiales no generen un costo al ser agregados, de esta manera, los materiales serán directamente agregados a la ficha técnica. El costo será calculado a partir de un total de los valores de estos materiales, y se asignará al costo que pertenece a materia prima directa o indirecta. Se presentó un problema con la base de datos, generó una lista de bugs inesperados y se tuvo que regenerar el código desde el repositorio en linea para poder seguir trabajando.</t>
+  </si>
+  <si>
+    <t>22/11/2015</t>
+  </si>
+  <si>
+    <t>Se expandió el modelo de datos, ahora los modelos cuentan con una propiedad llamada FichaTecnica, la cuál se compone de una entidad que agrupa un departamento con una lista de materiales, cada material contiene su consumo por par y su costo total, el cuál es calculado multiplicando el costo unitario con el consumo por par.</t>
+  </si>
+  <si>
+    <t>23/11/2015</t>
+  </si>
+  <si>
+    <t>Se listan los departamentos de produccion en la ficha tecnica, la vista fue modificada y se permitira agregar los materiales a la ficha</t>
+  </si>
+  <si>
+    <t>24/11/2015</t>
+  </si>
+  <si>
+    <t>Se trabajó con la vista que permitirá añadir los materiales a la ficha técnica, se configuró la tabla para mostrar los materiales</t>
+  </si>
+  <si>
+    <t>25/11/2015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El front-end de la vista calcula el costo total a partir del consumo y el costo unitario, se abre un diálogo para introducir los datos del material. Se envia una petición AJAX al servidor con la información del costo del material y su consumo para que sea guardado en la BD. </t>
+  </si>
+  <si>
+    <t>28/11/2015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se guarda correctamente el material en la ficha técnica. La vista ahora permite mostrar los materiales agregados. Se modificó el formulario de agregar para que muestre mejor los datos. También se modificó la base de datos para no incluir más de 2 digitos luego de la coma en algunas propiedades. </t>
+  </si>
+  <si>
+    <t>29/11/2015</t>
+  </si>
+  <si>
+    <t>Se agregó la funcionalidad para eliminar los materiales, ya sea por haberlo repetido o por otra razón. Se permite agregar materiales repetidos debido a que no hay forma de mapear un CostoMaterial con un Material sin añadir mucha complejidad al código</t>
+  </si>
+  <si>
+    <t>Al añadir un nuevo departamento, éste se añade automaticamente a la ficha técnica de todos los modelos. Ahora se muestra el costo por materia prima directa e indirecta en la ficha técnica</t>
   </si>
 </sst>
 </file>
@@ -275,7 +314,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -306,6 +345,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -319,7 +364,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -372,18 +417,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -392,23 +431,47 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -690,10 +753,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M69"/>
+  <dimension ref="A1:M88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E62" sqref="E62:I64"/>
+    <sheetView tabSelected="1" topLeftCell="A48" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M60" sqref="M60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -715,348 +778,348 @@
       <c r="G1" s="1"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="18"/>
+      <c r="B3" s="21"/>
       <c r="C3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="D3" s="21" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="18"/>
-      <c r="B4" s="18"/>
+      <c r="A4" s="21"/>
+      <c r="B4" s="21"/>
       <c r="C4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18" t="s">
+      <c r="D4" s="21"/>
+      <c r="E4" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="21"/>
     </row>
     <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="21"/>
-      <c r="C5" s="18" t="s">
+      <c r="B5" s="24"/>
+      <c r="C5" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="18">
-        <v>4</v>
-      </c>
-      <c r="E5" s="19" t="s">
+      <c r="D5" s="21">
+        <v>4</v>
+      </c>
+      <c r="E5" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="19"/>
-      <c r="G5" s="19"/>
-      <c r="H5" s="19"/>
-      <c r="I5" s="19"/>
+      <c r="F5" s="28"/>
+      <c r="G5" s="28"/>
+      <c r="H5" s="28"/>
+      <c r="I5" s="28"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="21"/>
-      <c r="B6" s="21"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="19"/>
-      <c r="I6" s="19"/>
+      <c r="A6" s="24"/>
+      <c r="B6" s="24"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="28"/>
+      <c r="I6" s="28"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="18"/>
-      <c r="C7" s="18" t="s">
+      <c r="B7" s="21"/>
+      <c r="C7" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="18">
-        <v>4</v>
-      </c>
-      <c r="E7" s="19" t="s">
+      <c r="D7" s="21">
+        <v>4</v>
+      </c>
+      <c r="E7" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="19"/>
-      <c r="G7" s="19"/>
-      <c r="H7" s="19"/>
-      <c r="I7" s="19"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="28"/>
+      <c r="H7" s="28"/>
+      <c r="I7" s="28"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="18"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="19"/>
-      <c r="F8" s="19"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="19"/>
-      <c r="I8" s="19"/>
+      <c r="A8" s="21"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="28"/>
+      <c r="I8" s="28"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="21">
+      <c r="A9" s="24">
         <v>42042</v>
       </c>
-      <c r="B9" s="21"/>
-      <c r="C9" s="18" t="s">
+      <c r="B9" s="24"/>
+      <c r="C9" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="18">
+      <c r="D9" s="21">
         <v>3</v>
       </c>
-      <c r="E9" s="19" t="s">
+      <c r="E9" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="F9" s="19"/>
-      <c r="G9" s="19"/>
-      <c r="H9" s="19"/>
-      <c r="I9" s="19"/>
+      <c r="F9" s="28"/>
+      <c r="G9" s="28"/>
+      <c r="H9" s="28"/>
+      <c r="I9" s="28"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="21"/>
-      <c r="B10" s="21"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="19"/>
-      <c r="I10" s="19"/>
+      <c r="A10" s="24"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="28"/>
+      <c r="H10" s="28"/>
+      <c r="I10" s="28"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="21">
+      <c r="A11" s="24">
         <v>42070</v>
       </c>
-      <c r="B11" s="18"/>
+      <c r="B11" s="21"/>
       <c r="C11" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D11" s="3">
         <v>3</v>
       </c>
-      <c r="E11" s="28" t="s">
+      <c r="E11" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="28"/>
-      <c r="G11" s="28"/>
-      <c r="H11" s="28"/>
-      <c r="I11" s="28"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="33"/>
+      <c r="H11" s="33"/>
+      <c r="I11" s="33"/>
     </row>
     <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="21">
+      <c r="A12" s="24">
         <v>42101</v>
       </c>
-      <c r="B12" s="21"/>
-      <c r="C12" s="18" t="s">
+      <c r="B12" s="24"/>
+      <c r="C12" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="18">
+      <c r="D12" s="21">
         <v>8</v>
       </c>
-      <c r="E12" s="19" t="s">
+      <c r="E12" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="F12" s="19"/>
-      <c r="G12" s="19"/>
-      <c r="H12" s="19"/>
-      <c r="I12" s="19"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="28"/>
+      <c r="H12" s="28"/>
+      <c r="I12" s="28"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="21"/>
-      <c r="B13" s="21"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="19"/>
-      <c r="F13" s="19"/>
-      <c r="G13" s="19"/>
-      <c r="H13" s="19"/>
-      <c r="I13" s="19"/>
+      <c r="A13" s="24"/>
+      <c r="B13" s="24"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="28"/>
+      <c r="G13" s="28"/>
+      <c r="H13" s="28"/>
+      <c r="I13" s="28"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="21"/>
-      <c r="B14" s="21"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="19"/>
-      <c r="F14" s="19"/>
-      <c r="G14" s="19"/>
-      <c r="H14" s="19"/>
-      <c r="I14" s="19"/>
+      <c r="A14" s="24"/>
+      <c r="B14" s="24"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="28"/>
+      <c r="H14" s="28"/>
+      <c r="I14" s="28"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="21">
+      <c r="A15" s="24">
         <v>42162</v>
       </c>
-      <c r="B15" s="18"/>
+      <c r="B15" s="21"/>
       <c r="C15" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D15" s="4">
         <v>4</v>
       </c>
-      <c r="E15" s="28" t="s">
+      <c r="E15" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="F15" s="28"/>
-      <c r="G15" s="28"/>
-      <c r="H15" s="28"/>
-      <c r="I15" s="28"/>
+      <c r="F15" s="33"/>
+      <c r="G15" s="33"/>
+      <c r="H15" s="33"/>
+      <c r="I15" s="33"/>
     </row>
     <row r="16" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="29">
+      <c r="A16" s="30">
         <v>42192</v>
       </c>
-      <c r="B16" s="29"/>
-      <c r="C16" s="31" t="s">
+      <c r="B16" s="30"/>
+      <c r="C16" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="D16" s="31">
-        <v>4</v>
-      </c>
-      <c r="E16" s="30" t="s">
+      <c r="D16" s="32">
+        <v>4</v>
+      </c>
+      <c r="E16" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="F16" s="30"/>
-      <c r="G16" s="30"/>
-      <c r="H16" s="30"/>
-      <c r="I16" s="30"/>
+      <c r="F16" s="31"/>
+      <c r="G16" s="31"/>
+      <c r="H16" s="31"/>
+      <c r="I16" s="31"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="29"/>
-      <c r="B17" s="29"/>
-      <c r="C17" s="31"/>
-      <c r="D17" s="31"/>
-      <c r="E17" s="30"/>
-      <c r="F17" s="30"/>
-      <c r="G17" s="30"/>
-      <c r="H17" s="30"/>
-      <c r="I17" s="30"/>
+      <c r="A17" s="30"/>
+      <c r="B17" s="30"/>
+      <c r="C17" s="32"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="31"/>
+      <c r="F17" s="31"/>
+      <c r="G17" s="31"/>
+      <c r="H17" s="31"/>
+      <c r="I17" s="31"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="29"/>
-      <c r="B18" s="29"/>
-      <c r="C18" s="31"/>
-      <c r="D18" s="31"/>
-      <c r="E18" s="30"/>
-      <c r="F18" s="30"/>
-      <c r="G18" s="30"/>
-      <c r="H18" s="30"/>
-      <c r="I18" s="30"/>
+      <c r="A18" s="30"/>
+      <c r="B18" s="30"/>
+      <c r="C18" s="32"/>
+      <c r="D18" s="32"/>
+      <c r="E18" s="31"/>
+      <c r="F18" s="31"/>
+      <c r="G18" s="31"/>
+      <c r="H18" s="31"/>
+      <c r="I18" s="31"/>
     </row>
     <row r="19" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="21">
+      <c r="A19" s="24">
         <v>42284</v>
       </c>
-      <c r="B19" s="21"/>
-      <c r="C19" s="18" t="s">
+      <c r="B19" s="24"/>
+      <c r="C19" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="D19" s="18">
-        <v>4</v>
-      </c>
-      <c r="E19" s="19" t="s">
+      <c r="D19" s="21">
+        <v>4</v>
+      </c>
+      <c r="E19" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="F19" s="19"/>
-      <c r="G19" s="19"/>
-      <c r="H19" s="19"/>
-      <c r="I19" s="19"/>
+      <c r="F19" s="28"/>
+      <c r="G19" s="28"/>
+      <c r="H19" s="28"/>
+      <c r="I19" s="28"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="21"/>
-      <c r="B20" s="21"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="19"/>
-      <c r="F20" s="19"/>
-      <c r="G20" s="19"/>
-      <c r="H20" s="19"/>
-      <c r="I20" s="19"/>
+      <c r="A20" s="24"/>
+      <c r="B20" s="24"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="28"/>
+      <c r="F20" s="28"/>
+      <c r="G20" s="28"/>
+      <c r="H20" s="28"/>
+      <c r="I20" s="28"/>
     </row>
     <row r="21" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="21">
+      <c r="A21" s="24">
         <v>42315</v>
       </c>
-      <c r="B21" s="21"/>
-      <c r="C21" s="18" t="s">
+      <c r="B21" s="24"/>
+      <c r="C21" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="D21" s="18">
-        <v>4</v>
-      </c>
-      <c r="E21" s="27" t="s">
+      <c r="D21" s="21">
+        <v>4</v>
+      </c>
+      <c r="E21" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="F21" s="27"/>
-      <c r="G21" s="27"/>
-      <c r="H21" s="27"/>
-      <c r="I21" s="27"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="20"/>
+      <c r="I21" s="20"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="21"/>
-      <c r="B22" s="21"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="27"/>
-      <c r="F22" s="27"/>
-      <c r="G22" s="27"/>
-      <c r="H22" s="27"/>
-      <c r="I22" s="27"/>
+      <c r="A22" s="24"/>
+      <c r="B22" s="24"/>
+      <c r="C22" s="21"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="20"/>
+      <c r="G22" s="20"/>
+      <c r="H22" s="20"/>
+      <c r="I22" s="20"/>
     </row>
     <row r="23" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="21">
+      <c r="A23" s="24">
         <v>42345</v>
       </c>
-      <c r="B23" s="21"/>
-      <c r="C23" s="18" t="s">
+      <c r="B23" s="24"/>
+      <c r="C23" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="D23" s="18">
+      <c r="D23" s="21">
         <v>8</v>
       </c>
-      <c r="E23" s="27" t="s">
+      <c r="E23" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="F23" s="27"/>
-      <c r="G23" s="27"/>
-      <c r="H23" s="27"/>
-      <c r="I23" s="27"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="20"/>
+      <c r="H23" s="20"/>
+      <c r="I23" s="20"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="21"/>
-      <c r="B24" s="21"/>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="27"/>
-      <c r="F24" s="27"/>
-      <c r="G24" s="27"/>
-      <c r="H24" s="27"/>
-      <c r="I24" s="27"/>
+      <c r="A24" s="24"/>
+      <c r="B24" s="24"/>
+      <c r="C24" s="21"/>
+      <c r="D24" s="21"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="20"/>
+      <c r="H24" s="20"/>
+      <c r="I24" s="20"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="21"/>
-      <c r="B25" s="21"/>
-      <c r="C25" s="18"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="27"/>
-      <c r="F25" s="27"/>
-      <c r="G25" s="27"/>
-      <c r="H25" s="27"/>
-      <c r="I25" s="27"/>
+      <c r="A25" s="24"/>
+      <c r="B25" s="24"/>
+      <c r="C25" s="21"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="20"/>
+      <c r="H25" s="20"/>
+      <c r="I25" s="20"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="18" t="s">
+      <c r="A26" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="18"/>
+      <c r="B26" s="21"/>
       <c r="C26" s="5" t="s">
         <v>6</v>
       </c>
@@ -1068,122 +1131,122 @@
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="18" t="s">
+      <c r="A27" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="18"/>
-      <c r="C27" s="18" t="s">
+      <c r="B27" s="21"/>
+      <c r="C27" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="D27" s="18">
-        <v>4</v>
-      </c>
-      <c r="E27" s="19" t="s">
+      <c r="D27" s="21">
+        <v>4</v>
+      </c>
+      <c r="E27" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="F27" s="19"/>
-      <c r="G27" s="19"/>
-      <c r="H27" s="19"/>
-      <c r="I27" s="19"/>
+      <c r="F27" s="28"/>
+      <c r="G27" s="28"/>
+      <c r="H27" s="28"/>
+      <c r="I27" s="28"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="18"/>
-      <c r="B28" s="18"/>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="19"/>
-      <c r="F28" s="19"/>
-      <c r="G28" s="19"/>
-      <c r="H28" s="19"/>
-      <c r="I28" s="19"/>
+      <c r="A28" s="21"/>
+      <c r="B28" s="21"/>
+      <c r="C28" s="21"/>
+      <c r="D28" s="21"/>
+      <c r="E28" s="28"/>
+      <c r="F28" s="28"/>
+      <c r="G28" s="28"/>
+      <c r="H28" s="28"/>
+      <c r="I28" s="28"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="18" t="s">
+      <c r="A29" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="B29" s="18"/>
-      <c r="C29" s="18" t="s">
+      <c r="B29" s="21"/>
+      <c r="C29" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="D29" s="18">
-        <v>4</v>
-      </c>
-      <c r="E29" s="19" t="s">
+      <c r="D29" s="21">
+        <v>4</v>
+      </c>
+      <c r="E29" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="F29" s="19"/>
-      <c r="G29" s="19"/>
-      <c r="H29" s="19"/>
-      <c r="I29" s="19"/>
+      <c r="F29" s="28"/>
+      <c r="G29" s="28"/>
+      <c r="H29" s="28"/>
+      <c r="I29" s="28"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="18"/>
-      <c r="B30" s="18"/>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="19"/>
-      <c r="F30" s="19"/>
-      <c r="G30" s="19"/>
-      <c r="H30" s="19"/>
-      <c r="I30" s="19"/>
+      <c r="A30" s="21"/>
+      <c r="B30" s="21"/>
+      <c r="C30" s="21"/>
+      <c r="D30" s="21"/>
+      <c r="E30" s="28"/>
+      <c r="F30" s="28"/>
+      <c r="G30" s="28"/>
+      <c r="H30" s="28"/>
+      <c r="I30" s="28"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="18" t="s">
+      <c r="A31" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="B31" s="18"/>
-      <c r="C31" s="18" t="s">
+      <c r="B31" s="21"/>
+      <c r="C31" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="D31" s="18">
+      <c r="D31" s="21">
         <v>8</v>
       </c>
-      <c r="E31" s="27" t="s">
+      <c r="E31" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="F31" s="27"/>
-      <c r="G31" s="27"/>
-      <c r="H31" s="27"/>
-      <c r="I31" s="27"/>
+      <c r="F31" s="20"/>
+      <c r="G31" s="20"/>
+      <c r="H31" s="20"/>
+      <c r="I31" s="20"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="18"/>
-      <c r="B32" s="18"/>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
-      <c r="E32" s="27"/>
-      <c r="F32" s="27"/>
-      <c r="G32" s="27"/>
-      <c r="H32" s="27"/>
-      <c r="I32" s="27"/>
+      <c r="A32" s="21"/>
+      <c r="B32" s="21"/>
+      <c r="C32" s="21"/>
+      <c r="D32" s="21"/>
+      <c r="E32" s="20"/>
+      <c r="F32" s="20"/>
+      <c r="G32" s="20"/>
+      <c r="H32" s="20"/>
+      <c r="I32" s="20"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="18"/>
-      <c r="B33" s="18"/>
-      <c r="C33" s="18"/>
-      <c r="D33" s="18"/>
-      <c r="E33" s="27"/>
-      <c r="F33" s="27"/>
-      <c r="G33" s="27"/>
-      <c r="H33" s="27"/>
-      <c r="I33" s="27"/>
+      <c r="A33" s="21"/>
+      <c r="B33" s="21"/>
+      <c r="C33" s="21"/>
+      <c r="D33" s="21"/>
+      <c r="E33" s="20"/>
+      <c r="F33" s="20"/>
+      <c r="G33" s="20"/>
+      <c r="H33" s="20"/>
+      <c r="I33" s="20"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="18"/>
-      <c r="B34" s="18"/>
-      <c r="C34" s="18"/>
-      <c r="D34" s="18"/>
-      <c r="E34" s="27"/>
-      <c r="F34" s="27"/>
-      <c r="G34" s="27"/>
-      <c r="H34" s="27"/>
-      <c r="I34" s="27"/>
+      <c r="A34" s="21"/>
+      <c r="B34" s="21"/>
+      <c r="C34" s="21"/>
+      <c r="D34" s="21"/>
+      <c r="E34" s="20"/>
+      <c r="F34" s="20"/>
+      <c r="G34" s="20"/>
+      <c r="H34" s="20"/>
+      <c r="I34" s="20"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="18" t="s">
+      <c r="A35" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="B35" s="18"/>
+      <c r="B35" s="21"/>
       <c r="C35" s="6" t="s">
         <v>16</v>
       </c>
@@ -1195,40 +1258,40 @@
       </c>
     </row>
     <row r="36" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="18" t="s">
+      <c r="A36" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="B36" s="18"/>
-      <c r="C36" s="18" t="s">
+      <c r="B36" s="21"/>
+      <c r="C36" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="D36" s="18">
+      <c r="D36" s="21">
         <v>8</v>
       </c>
-      <c r="E36" s="27" t="s">
+      <c r="E36" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="F36" s="27"/>
-      <c r="G36" s="27"/>
-      <c r="H36" s="27"/>
-      <c r="I36" s="27"/>
+      <c r="F36" s="20"/>
+      <c r="G36" s="20"/>
+      <c r="H36" s="20"/>
+      <c r="I36" s="20"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="18"/>
-      <c r="B37" s="18"/>
-      <c r="C37" s="18"/>
-      <c r="D37" s="18"/>
-      <c r="E37" s="27"/>
-      <c r="F37" s="27"/>
-      <c r="G37" s="27"/>
-      <c r="H37" s="27"/>
-      <c r="I37" s="27"/>
+      <c r="A37" s="21"/>
+      <c r="B37" s="21"/>
+      <c r="C37" s="21"/>
+      <c r="D37" s="21"/>
+      <c r="E37" s="20"/>
+      <c r="F37" s="20"/>
+      <c r="G37" s="20"/>
+      <c r="H37" s="20"/>
+      <c r="I37" s="20"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="18" t="s">
+      <c r="A38" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="B38" s="18"/>
+      <c r="B38" s="21"/>
       <c r="C38" s="7" t="s">
         <v>6</v>
       </c>
@@ -1240,40 +1303,40 @@
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="18" t="s">
+      <c r="A39" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="B39" s="18"/>
-      <c r="C39" s="18" t="s">
+      <c r="B39" s="21"/>
+      <c r="C39" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="D39" s="18">
-        <v>4</v>
-      </c>
-      <c r="E39" s="27" t="s">
+      <c r="D39" s="21">
+        <v>4</v>
+      </c>
+      <c r="E39" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="F39" s="27"/>
-      <c r="G39" s="27"/>
-      <c r="H39" s="27"/>
-      <c r="I39" s="27"/>
+      <c r="F39" s="20"/>
+      <c r="G39" s="20"/>
+      <c r="H39" s="20"/>
+      <c r="I39" s="20"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="18"/>
-      <c r="B40" s="18"/>
-      <c r="C40" s="18"/>
-      <c r="D40" s="18"/>
-      <c r="E40" s="27"/>
-      <c r="F40" s="27"/>
-      <c r="G40" s="27"/>
-      <c r="H40" s="27"/>
-      <c r="I40" s="27"/>
+      <c r="A40" s="21"/>
+      <c r="B40" s="21"/>
+      <c r="C40" s="21"/>
+      <c r="D40" s="21"/>
+      <c r="E40" s="20"/>
+      <c r="F40" s="20"/>
+      <c r="G40" s="20"/>
+      <c r="H40" s="20"/>
+      <c r="I40" s="20"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="18" t="s">
+      <c r="A41" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="B41" s="18"/>
+      <c r="B41" s="21"/>
       <c r="C41" s="8" t="s">
         <v>6</v>
       </c>
@@ -1285,10 +1348,10 @@
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="18" t="s">
+      <c r="A42" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="B42" s="18"/>
+      <c r="B42" s="21"/>
       <c r="C42" s="8" t="s">
         <v>10</v>
       </c>
@@ -1300,10 +1363,10 @@
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" s="18" t="s">
+      <c r="A43" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="B43" s="18"/>
+      <c r="B43" s="21"/>
       <c r="C43" s="8" t="s">
         <v>14</v>
       </c>
@@ -1315,10 +1378,10 @@
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="18" t="s">
+      <c r="A44" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="B44" s="18"/>
+      <c r="B44" s="21"/>
       <c r="C44" s="8" t="s">
         <v>16</v>
       </c>
@@ -1330,10 +1393,10 @@
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" s="18" t="s">
+      <c r="A45" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="B45" s="18"/>
+      <c r="B45" s="21"/>
       <c r="C45" s="9" t="s">
         <v>10</v>
       </c>
@@ -1345,10 +1408,10 @@
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" s="26" t="s">
+      <c r="A46" s="34" t="s">
         <v>51</v>
       </c>
-      <c r="B46" s="26"/>
+      <c r="B46" s="34"/>
       <c r="C46" s="12" t="s">
         <v>14</v>
       </c>
@@ -1364,113 +1427,113 @@
       <c r="I46" s="13"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47" s="25" t="s">
+      <c r="A47" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="B47" s="25"/>
-      <c r="C47" s="25" t="s">
+      <c r="B47" s="23"/>
+      <c r="C47" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="D47" s="25">
-        <v>4</v>
-      </c>
-      <c r="E47" s="24" t="s">
+      <c r="D47" s="23">
+        <v>4</v>
+      </c>
+      <c r="E47" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="F47" s="24"/>
-      <c r="G47" s="24"/>
-      <c r="H47" s="24"/>
-      <c r="I47" s="24"/>
+      <c r="F47" s="22"/>
+      <c r="G47" s="22"/>
+      <c r="H47" s="22"/>
+      <c r="I47" s="22"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" s="25"/>
-      <c r="B48" s="25"/>
-      <c r="C48" s="25"/>
-      <c r="D48" s="25"/>
-      <c r="E48" s="24"/>
-      <c r="F48" s="24"/>
-      <c r="G48" s="24"/>
-      <c r="H48" s="24"/>
-      <c r="I48" s="24"/>
+      <c r="A48" s="23"/>
+      <c r="B48" s="23"/>
+      <c r="C48" s="23"/>
+      <c r="D48" s="23"/>
+      <c r="E48" s="22"/>
+      <c r="F48" s="22"/>
+      <c r="G48" s="22"/>
+      <c r="H48" s="22"/>
+      <c r="I48" s="22"/>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A49" s="21">
+      <c r="A49" s="24">
         <v>42134</v>
       </c>
-      <c r="B49" s="21"/>
-      <c r="C49" s="20" t="s">
+      <c r="B49" s="24"/>
+      <c r="C49" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="D49" s="20">
-        <v>4</v>
-      </c>
-      <c r="E49" s="19" t="s">
+      <c r="D49" s="29">
+        <v>4</v>
+      </c>
+      <c r="E49" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="F49" s="19"/>
-      <c r="G49" s="19"/>
-      <c r="H49" s="19"/>
-      <c r="I49" s="19"/>
+      <c r="F49" s="28"/>
+      <c r="G49" s="28"/>
+      <c r="H49" s="28"/>
+      <c r="I49" s="28"/>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A50" s="21"/>
-      <c r="B50" s="21"/>
-      <c r="C50" s="20"/>
-      <c r="D50" s="20"/>
-      <c r="E50" s="19"/>
-      <c r="F50" s="19"/>
-      <c r="G50" s="19"/>
-      <c r="H50" s="19"/>
-      <c r="I50" s="19"/>
-      <c r="L50" s="23" t="s">
+      <c r="A50" s="24"/>
+      <c r="B50" s="24"/>
+      <c r="C50" s="29"/>
+      <c r="D50" s="29"/>
+      <c r="E50" s="28"/>
+      <c r="F50" s="28"/>
+      <c r="G50" s="28"/>
+      <c r="H50" s="28"/>
+      <c r="I50" s="28"/>
+      <c r="L50" s="36" t="s">
         <v>55</v>
       </c>
-      <c r="M50" s="23"/>
+      <c r="M50" s="36"/>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A51" s="21">
+      <c r="A51" s="24">
         <v>42165</v>
       </c>
-      <c r="B51" s="21"/>
-      <c r="C51" s="20" t="s">
+      <c r="B51" s="24"/>
+      <c r="C51" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="D51" s="20">
+      <c r="D51" s="29">
         <v>8</v>
       </c>
-      <c r="E51" s="19" t="s">
+      <c r="E51" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="F51" s="19"/>
-      <c r="G51" s="19"/>
-      <c r="H51" s="19"/>
-      <c r="I51" s="19"/>
-      <c r="L51" s="22">
-        <f>SUM(D5:D69)</f>
-        <v>183</v>
-      </c>
-      <c r="M51" s="22"/>
+      <c r="F51" s="28"/>
+      <c r="G51" s="28"/>
+      <c r="H51" s="28"/>
+      <c r="I51" s="28"/>
+      <c r="L51" s="35">
+        <f>SUM(D5:D85)</f>
+        <v>217</v>
+      </c>
+      <c r="M51" s="35"/>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A52" s="21"/>
-      <c r="B52" s="21"/>
-      <c r="C52" s="20"/>
-      <c r="D52" s="20"/>
-      <c r="E52" s="19"/>
-      <c r="F52" s="19"/>
-      <c r="G52" s="19"/>
-      <c r="H52" s="19"/>
-      <c r="I52" s="19"/>
-      <c r="L52" s="23" t="s">
+      <c r="A52" s="24"/>
+      <c r="B52" s="24"/>
+      <c r="C52" s="29"/>
+      <c r="D52" s="29"/>
+      <c r="E52" s="28"/>
+      <c r="F52" s="28"/>
+      <c r="G52" s="28"/>
+      <c r="H52" s="28"/>
+      <c r="I52" s="28"/>
+      <c r="L52" s="36" t="s">
         <v>56</v>
       </c>
-      <c r="M52" s="23"/>
+      <c r="M52" s="36"/>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A53" s="18" t="s">
+      <c r="A53" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="B53" s="18"/>
+      <c r="B53" s="21"/>
       <c r="C53" s="10" t="s">
         <v>12</v>
       </c>
@@ -1480,17 +1543,17 @@
       <c r="E53" t="s">
         <v>62</v>
       </c>
-      <c r="L53" s="22">
+      <c r="L53" s="35">
         <f>SUM(D5:D48)</f>
         <v>119</v>
       </c>
-      <c r="M53" s="22"/>
+      <c r="M53" s="35"/>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A54" s="18" t="s">
+      <c r="A54" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="B54" s="18"/>
+      <c r="B54" s="21"/>
       <c r="C54" s="10" t="s">
         <v>14</v>
       </c>
@@ -1500,16 +1563,16 @@
       <c r="E54" t="s">
         <v>63</v>
       </c>
-      <c r="L54" s="23" t="s">
+      <c r="L54" s="36" t="s">
         <v>57</v>
       </c>
-      <c r="M54" s="23"/>
+      <c r="M54" s="36"/>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A55" s="18" t="s">
+      <c r="A55" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="B55" s="18"/>
+      <c r="B55" s="21"/>
       <c r="C55" s="11" t="s">
         <v>14</v>
       </c>
@@ -1519,47 +1582,47 @@
       <c r="E55" t="s">
         <v>64</v>
       </c>
-      <c r="L55" s="22">
-        <f>SUM(D49:D69)</f>
-        <v>64</v>
-      </c>
-      <c r="M55" s="22"/>
+      <c r="L55" s="35">
+        <f>SUM(D73:D85)</f>
+        <v>32</v>
+      </c>
+      <c r="M55" s="35"/>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A56" s="21">
+      <c r="A56" s="24">
         <v>42166</v>
       </c>
-      <c r="B56" s="21"/>
-      <c r="C56" s="20" t="s">
+      <c r="B56" s="24"/>
+      <c r="C56" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="D56" s="20">
+      <c r="D56" s="29">
         <v>8</v>
       </c>
-      <c r="E56" s="19" t="s">
+      <c r="E56" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="F56" s="19"/>
-      <c r="G56" s="19"/>
-      <c r="H56" s="19"/>
-      <c r="I56" s="19"/>
+      <c r="F56" s="28"/>
+      <c r="G56" s="28"/>
+      <c r="H56" s="28"/>
+      <c r="I56" s="28"/>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A57" s="21"/>
-      <c r="B57" s="21"/>
-      <c r="C57" s="20"/>
-      <c r="D57" s="20"/>
-      <c r="E57" s="19"/>
-      <c r="F57" s="19"/>
-      <c r="G57" s="19"/>
-      <c r="H57" s="19"/>
-      <c r="I57" s="19"/>
+      <c r="A57" s="24"/>
+      <c r="B57" s="24"/>
+      <c r="C57" s="29"/>
+      <c r="D57" s="29"/>
+      <c r="E57" s="28"/>
+      <c r="F57" s="28"/>
+      <c r="G57" s="28"/>
+      <c r="H57" s="28"/>
+      <c r="I57" s="28"/>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A58" s="21">
+      <c r="A58" s="24">
         <v>42196</v>
       </c>
-      <c r="B58" s="21"/>
+      <c r="B58" s="24"/>
       <c r="C58" s="14" t="s">
         <v>16</v>
       </c>
@@ -1571,10 +1634,10 @@
       </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A59" s="21">
+      <c r="A59" s="24">
         <v>42227</v>
       </c>
-      <c r="B59" s="21"/>
+      <c r="B59" s="24"/>
       <c r="C59" s="15" t="s">
         <v>23</v>
       </c>
@@ -1586,10 +1649,10 @@
       </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A60" s="21">
+      <c r="A60" s="24">
         <v>42288</v>
       </c>
-      <c r="B60" s="21"/>
+      <c r="B60" s="24"/>
       <c r="C60" s="16" t="s">
         <v>10</v>
       </c>
@@ -1601,10 +1664,10 @@
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A61" s="18" t="s">
+      <c r="A61" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="B61" s="18"/>
+      <c r="B61" s="21"/>
       <c r="C61" s="17" t="s">
         <v>14</v>
       </c>
@@ -1616,154 +1679,387 @@
       </c>
     </row>
     <row r="62" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="18" t="s">
+      <c r="A62" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="B62" s="18"/>
-      <c r="C62" s="20" t="s">
+      <c r="B62" s="21"/>
+      <c r="C62" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="D62" s="20">
+      <c r="D62" s="29">
         <v>6</v>
       </c>
-      <c r="E62" s="19" t="s">
+      <c r="E62" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="F62" s="19"/>
-      <c r="G62" s="19"/>
-      <c r="H62" s="19"/>
-      <c r="I62" s="19"/>
+      <c r="F62" s="28"/>
+      <c r="G62" s="28"/>
+      <c r="H62" s="28"/>
+      <c r="I62" s="28"/>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A63" s="18"/>
-      <c r="B63" s="18"/>
-      <c r="C63" s="20"/>
-      <c r="D63" s="20"/>
-      <c r="E63" s="19"/>
-      <c r="F63" s="19"/>
-      <c r="G63" s="19"/>
-      <c r="H63" s="19"/>
-      <c r="I63" s="19"/>
+      <c r="A63" s="21"/>
+      <c r="B63" s="21"/>
+      <c r="C63" s="29"/>
+      <c r="D63" s="29"/>
+      <c r="E63" s="28"/>
+      <c r="F63" s="28"/>
+      <c r="G63" s="28"/>
+      <c r="H63" s="28"/>
+      <c r="I63" s="28"/>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A64" s="18"/>
-      <c r="B64" s="18"/>
-      <c r="C64" s="20"/>
-      <c r="D64" s="20"/>
-      <c r="E64" s="19"/>
-      <c r="F64" s="19"/>
-      <c r="G64" s="19"/>
-      <c r="H64" s="19"/>
-      <c r="I64" s="19"/>
+      <c r="A64" s="21"/>
+      <c r="B64" s="21"/>
+      <c r="C64" s="29"/>
+      <c r="D64" s="29"/>
+      <c r="E64" s="28"/>
+      <c r="F64" s="28"/>
+      <c r="G64" s="28"/>
+      <c r="H64" s="28"/>
+      <c r="I64" s="28"/>
     </row>
     <row r="65" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="18" t="s">
+      <c r="A65" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="B65" s="18"/>
-      <c r="C65" s="20" t="s">
+      <c r="B65" s="21"/>
+      <c r="C65" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="D65" s="20">
+      <c r="D65" s="29">
+        <v>6</v>
+      </c>
+      <c r="E65" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="F65" s="28"/>
+      <c r="G65" s="28"/>
+      <c r="H65" s="28"/>
+      <c r="I65" s="28"/>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A66" s="21"/>
+      <c r="B66" s="21"/>
+      <c r="C66" s="29"/>
+      <c r="D66" s="29"/>
+      <c r="E66" s="28"/>
+      <c r="F66" s="28"/>
+      <c r="G66" s="28"/>
+      <c r="H66" s="28"/>
+      <c r="I66" s="28"/>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A67" s="21"/>
+      <c r="B67" s="21"/>
+      <c r="C67" s="29"/>
+      <c r="D67" s="29"/>
+      <c r="E67" s="28"/>
+      <c r="F67" s="28"/>
+      <c r="G67" s="28"/>
+      <c r="H67" s="28"/>
+      <c r="I67" s="28"/>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A68" s="21"/>
+      <c r="B68" s="21"/>
+      <c r="C68" s="29"/>
+      <c r="D68" s="29"/>
+      <c r="E68" s="28"/>
+      <c r="F68" s="28"/>
+      <c r="G68" s="28"/>
+      <c r="H68" s="28"/>
+      <c r="I68" s="28"/>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A69" s="21"/>
+      <c r="B69" s="21"/>
+      <c r="C69" s="29"/>
+      <c r="D69" s="29"/>
+      <c r="E69" s="28"/>
+      <c r="F69" s="28"/>
+      <c r="G69" s="28"/>
+      <c r="H69" s="28"/>
+      <c r="I69" s="28"/>
+    </row>
+    <row r="70" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="B70" s="27"/>
+      <c r="C70" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="D70" s="26">
+        <v>4</v>
+      </c>
+      <c r="E70" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="F70" s="25"/>
+      <c r="G70" s="25"/>
+      <c r="H70" s="25"/>
+      <c r="I70" s="25"/>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A71" s="27"/>
+      <c r="B71" s="27"/>
+      <c r="C71" s="26"/>
+      <c r="D71" s="26"/>
+      <c r="E71" s="25"/>
+      <c r="F71" s="25"/>
+      <c r="G71" s="25"/>
+      <c r="H71" s="25"/>
+      <c r="I71" s="25"/>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A72" s="27"/>
+      <c r="B72" s="27"/>
+      <c r="C72" s="26"/>
+      <c r="D72" s="26"/>
+      <c r="E72" s="25"/>
+      <c r="F72" s="25"/>
+      <c r="G72" s="25"/>
+      <c r="H72" s="25"/>
+      <c r="I72" s="25"/>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A73" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="B73" s="21"/>
+      <c r="C73" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="D73" s="18">
+        <v>4</v>
+      </c>
+      <c r="E73" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A74" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="B74" s="21"/>
+      <c r="C74" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D74" s="19">
+        <v>4</v>
+      </c>
+      <c r="E74" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A75" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="B75" s="21"/>
+      <c r="C75" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="D75" s="21">
         <v>8</v>
       </c>
-      <c r="E65" s="19" t="s">
-        <v>75</v>
-      </c>
-      <c r="F65" s="19"/>
-      <c r="G65" s="19"/>
-      <c r="H65" s="19"/>
-      <c r="I65" s="19"/>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A66" s="18"/>
-      <c r="B66" s="18"/>
-      <c r="C66" s="20"/>
-      <c r="D66" s="20"/>
-      <c r="E66" s="19"/>
-      <c r="F66" s="19"/>
-      <c r="G66" s="19"/>
-      <c r="H66" s="19"/>
-      <c r="I66" s="19"/>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A67" s="18"/>
-      <c r="B67" s="18"/>
-      <c r="C67" s="20"/>
-      <c r="D67" s="20"/>
-      <c r="E67" s="19"/>
-      <c r="F67" s="19"/>
-      <c r="G67" s="19"/>
-      <c r="H67" s="19"/>
-      <c r="I67" s="19"/>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A68" s="18"/>
-      <c r="B68" s="18"/>
-      <c r="C68" s="20"/>
-      <c r="D68" s="20"/>
-      <c r="E68" s="19"/>
-      <c r="F68" s="19"/>
-      <c r="G68" s="19"/>
-      <c r="H68" s="19"/>
-      <c r="I68" s="19"/>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A69" s="18"/>
-      <c r="B69" s="18"/>
-      <c r="C69" s="20"/>
-      <c r="D69" s="20"/>
-      <c r="E69" s="19"/>
-      <c r="F69" s="19"/>
-      <c r="G69" s="19"/>
-      <c r="H69" s="19"/>
-      <c r="I69" s="19"/>
+      <c r="E75" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="F75" s="20"/>
+      <c r="G75" s="20"/>
+      <c r="H75" s="20"/>
+      <c r="I75" s="20"/>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A76" s="21"/>
+      <c r="B76" s="21"/>
+      <c r="C76" s="21"/>
+      <c r="D76" s="21"/>
+      <c r="E76" s="20"/>
+      <c r="F76" s="20"/>
+      <c r="G76" s="20"/>
+      <c r="H76" s="20"/>
+      <c r="I76" s="20"/>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A77" s="21"/>
+      <c r="B77" s="21"/>
+      <c r="C77" s="21"/>
+      <c r="D77" s="21"/>
+      <c r="E77" s="20"/>
+      <c r="F77" s="20"/>
+      <c r="G77" s="20"/>
+      <c r="H77" s="20"/>
+      <c r="I77" s="20"/>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A78" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="B78" s="21"/>
+      <c r="C78" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="D78" s="21">
+        <v>8</v>
+      </c>
+      <c r="E78" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="F78" s="20"/>
+      <c r="G78" s="20"/>
+      <c r="H78" s="20"/>
+      <c r="I78" s="20"/>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A79" s="21"/>
+      <c r="B79" s="21"/>
+      <c r="C79" s="21"/>
+      <c r="D79" s="21"/>
+      <c r="E79" s="20"/>
+      <c r="F79" s="20"/>
+      <c r="G79" s="20"/>
+      <c r="H79" s="20"/>
+      <c r="I79" s="20"/>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A80" s="21"/>
+      <c r="B80" s="21"/>
+      <c r="C80" s="21"/>
+      <c r="D80" s="21"/>
+      <c r="E80" s="20"/>
+      <c r="F80" s="20"/>
+      <c r="G80" s="20"/>
+      <c r="H80" s="20"/>
+      <c r="I80" s="20"/>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A81" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="B81" s="21"/>
+      <c r="C81" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="D81" s="21">
+        <v>4</v>
+      </c>
+      <c r="E81" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="F81" s="20"/>
+      <c r="G81" s="20"/>
+      <c r="H81" s="20"/>
+      <c r="I81" s="20"/>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A82" s="21"/>
+      <c r="B82" s="21"/>
+      <c r="C82" s="21"/>
+      <c r="D82" s="21"/>
+      <c r="E82" s="20"/>
+      <c r="F82" s="20"/>
+      <c r="G82" s="20"/>
+      <c r="H82" s="20"/>
+      <c r="I82" s="20"/>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A83" s="21"/>
+      <c r="B83" s="21"/>
+      <c r="C83" s="21"/>
+      <c r="D83" s="21"/>
+      <c r="E83" s="20"/>
+      <c r="F83" s="20"/>
+      <c r="G83" s="20"/>
+      <c r="H83" s="20"/>
+      <c r="I83" s="20"/>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A84" s="24">
+        <v>42016</v>
+      </c>
+      <c r="B84" s="24"/>
+      <c r="C84" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D84" s="21">
+        <v>4</v>
+      </c>
+      <c r="E84" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="F84" s="20"/>
+      <c r="G84" s="20"/>
+      <c r="H84" s="20"/>
+      <c r="I84" s="20"/>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A85" s="24"/>
+      <c r="B85" s="24"/>
+      <c r="C85" s="21"/>
+      <c r="D85" s="21"/>
+      <c r="E85" s="20"/>
+      <c r="F85" s="20"/>
+      <c r="G85" s="20"/>
+      <c r="H85" s="20"/>
+      <c r="I85" s="20"/>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F88" s="37"/>
     </row>
   </sheetData>
-  <mergeCells count="105">
-    <mergeCell ref="E65:I69"/>
-    <mergeCell ref="D65:D69"/>
-    <mergeCell ref="C65:C69"/>
-    <mergeCell ref="A65:B69"/>
-    <mergeCell ref="E62:I64"/>
-    <mergeCell ref="D62:D64"/>
-    <mergeCell ref="C62:C64"/>
-    <mergeCell ref="A62:B64"/>
-    <mergeCell ref="E29:I30"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="E39:I40"/>
-    <mergeCell ref="A29:B30"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A36:B37"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="C39:C40"/>
-    <mergeCell ref="E31:I34"/>
-    <mergeCell ref="D31:D34"/>
-    <mergeCell ref="C31:C34"/>
-    <mergeCell ref="A31:B34"/>
+  <mergeCells count="127">
+    <mergeCell ref="E84:I85"/>
+    <mergeCell ref="D84:D85"/>
+    <mergeCell ref="C84:C85"/>
+    <mergeCell ref="A84:B85"/>
+    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="E75:I77"/>
+    <mergeCell ref="D75:D77"/>
+    <mergeCell ref="C75:C77"/>
+    <mergeCell ref="A75:B77"/>
+    <mergeCell ref="E78:I80"/>
+    <mergeCell ref="D78:D80"/>
+    <mergeCell ref="C78:C80"/>
+    <mergeCell ref="A78:B80"/>
+    <mergeCell ref="L55:M55"/>
+    <mergeCell ref="L50:M50"/>
+    <mergeCell ref="L51:M51"/>
+    <mergeCell ref="L52:M52"/>
+    <mergeCell ref="L53:M53"/>
+    <mergeCell ref="L54:M54"/>
+    <mergeCell ref="E51:I52"/>
+    <mergeCell ref="D51:D52"/>
+    <mergeCell ref="C51:C52"/>
+    <mergeCell ref="E49:I50"/>
+    <mergeCell ref="D49:D50"/>
+    <mergeCell ref="C49:C50"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="E27:I28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="A27:B28"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="E56:I57"/>
+    <mergeCell ref="D56:D57"/>
+    <mergeCell ref="C56:C57"/>
+    <mergeCell ref="A56:B57"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="E36:I37"/>
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="A39:B40"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A51:B52"/>
+    <mergeCell ref="A49:B50"/>
     <mergeCell ref="A53:B53"/>
     <mergeCell ref="A54:B54"/>
-    <mergeCell ref="A51:B52"/>
-    <mergeCell ref="A49:B50"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="A16:B18"/>
-    <mergeCell ref="E23:I25"/>
-    <mergeCell ref="D23:D25"/>
-    <mergeCell ref="C23:C25"/>
-    <mergeCell ref="A23:B25"/>
-    <mergeCell ref="E16:I18"/>
-    <mergeCell ref="D16:D18"/>
-    <mergeCell ref="C16:C18"/>
-    <mergeCell ref="E19:I20"/>
-    <mergeCell ref="A21:B22"/>
-    <mergeCell ref="A19:B20"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="E21:I22"/>
-    <mergeCell ref="D21:D22"/>
     <mergeCell ref="E7:I8"/>
     <mergeCell ref="D7:D8"/>
     <mergeCell ref="C7:C8"/>
@@ -1787,45 +2083,61 @@
     <mergeCell ref="C12:C14"/>
     <mergeCell ref="A12:B14"/>
     <mergeCell ref="E9:I10"/>
+    <mergeCell ref="A16:B18"/>
+    <mergeCell ref="E23:I25"/>
+    <mergeCell ref="D23:D25"/>
+    <mergeCell ref="C23:C25"/>
+    <mergeCell ref="A23:B25"/>
+    <mergeCell ref="E16:I18"/>
+    <mergeCell ref="D16:D18"/>
+    <mergeCell ref="C16:C18"/>
+    <mergeCell ref="E19:I20"/>
+    <mergeCell ref="A21:B22"/>
+    <mergeCell ref="A19:B20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="E21:I22"/>
+    <mergeCell ref="D21:D22"/>
     <mergeCell ref="C21:C22"/>
+    <mergeCell ref="A62:B64"/>
+    <mergeCell ref="E29:I30"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="E39:I40"/>
+    <mergeCell ref="A29:B30"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A36:B37"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="E31:I34"/>
+    <mergeCell ref="D31:D34"/>
+    <mergeCell ref="C31:C34"/>
+    <mergeCell ref="A31:B34"/>
+    <mergeCell ref="E81:I83"/>
+    <mergeCell ref="D81:D83"/>
+    <mergeCell ref="C81:C83"/>
+    <mergeCell ref="A81:B83"/>
     <mergeCell ref="E47:I48"/>
     <mergeCell ref="D47:D48"/>
     <mergeCell ref="C47:C48"/>
     <mergeCell ref="A47:B48"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="E36:I37"/>
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="C36:C37"/>
-    <mergeCell ref="A39:B40"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="E27:I28"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="A27:B28"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="E56:I57"/>
-    <mergeCell ref="D56:D57"/>
-    <mergeCell ref="C56:C57"/>
-    <mergeCell ref="A56:B57"/>
+    <mergeCell ref="A73:B73"/>
     <mergeCell ref="A60:B60"/>
     <mergeCell ref="A58:B58"/>
-    <mergeCell ref="L55:M55"/>
-    <mergeCell ref="L50:M50"/>
-    <mergeCell ref="L51:M51"/>
-    <mergeCell ref="L52:M52"/>
-    <mergeCell ref="L53:M53"/>
-    <mergeCell ref="L54:M54"/>
-    <mergeCell ref="E51:I52"/>
-    <mergeCell ref="D51:D52"/>
-    <mergeCell ref="C51:C52"/>
-    <mergeCell ref="E49:I50"/>
-    <mergeCell ref="D49:D50"/>
-    <mergeCell ref="C49:C50"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="E70:I72"/>
+    <mergeCell ref="D70:D72"/>
+    <mergeCell ref="C70:C72"/>
+    <mergeCell ref="A70:B72"/>
+    <mergeCell ref="E65:I69"/>
+    <mergeCell ref="D65:D69"/>
+    <mergeCell ref="C65:C69"/>
+    <mergeCell ref="A65:B69"/>
+    <mergeCell ref="E62:I64"/>
+    <mergeCell ref="D62:D64"/>
+    <mergeCell ref="C62:C64"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>